<commit_message>
read uses constructor if available
</commit_message>
<xml_diff>
--- a/DaoGenerator/performance/performance-data.xlsx
+++ b/DaoGenerator/performance/performance-data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="19">
   <si>
     <t>100x Insert (one-by-one)</t>
   </si>
@@ -55,13 +55,31 @@
   </si>
   <si>
     <t>Load Factor</t>
+  </si>
+  <si>
+    <t>Load all 1000 (setters)</t>
+  </si>
+  <si>
+    <t>Load all 1000 (constructor)</t>
+  </si>
+  <si>
+    <t>Load/s (setters)</t>
+  </si>
+  <si>
+    <t>Load Factor (setters)</t>
+  </si>
+  <si>
+    <t>greenDAO vs. ORMLite</t>
+  </si>
+  <si>
+    <t>Load constructor vs. setters:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -73,6 +91,21 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.249977111117893"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -98,7 +131,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -107,10 +140,13 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -222,7 +258,7 @@
                   <c:v>5376.3440860215051</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6501.9505851755521</c:v>
+                  <c:v>8635.5785837651129</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -289,12 +325,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="47169024"/>
-        <c:axId val="93442560"/>
+        <c:axId val="158910976"/>
+        <c:axId val="154283392"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="47169024"/>
+        <c:axId val="158910976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -303,7 +339,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="93442560"/>
+        <c:crossAx val="154283392"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -311,7 +347,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="93442560"/>
+        <c:axId val="154283392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -322,7 +358,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="47169024"/>
+        <c:crossAx val="158910976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -666,89 +702,99 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="12.85546875" customWidth="1"/>
-    <col min="3" max="3" width="14" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" customWidth="1"/>
-    <col min="5" max="5" width="13.140625" customWidth="1"/>
-    <col min="6" max="6" width="8.7109375" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" style="1"/>
+    <col min="2" max="2" width="12.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="14" style="1" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="8.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="13" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="B1" s="4" t="s">
+    <row r="1" spans="1:7" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="G1" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="1">
         <f>greenDAO!B7</f>
         <v>7912.6</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="1">
         <f>greenDAO!C7</f>
         <v>817.6</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="1">
         <f>greenDAO!D7</f>
         <v>207.2</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="1">
         <f>greenDAO!E7</f>
         <v>186</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="1">
+        <f>greenDAO!G7</f>
+        <v>115.8</v>
+      </c>
+      <c r="G2" s="5">
         <f>greenDAO!F7</f>
         <v>153.80000000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="1">
         <f>ORMLite!B7</f>
         <v>8422.7999999999993</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="1">
         <f>ORMLite!C7</f>
         <v>8430.6</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="1">
         <f>ORMLite!D7</f>
         <v>449.8</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="1">
         <f>ORMLite!E7</f>
         <v>456.6</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="1">
         <f>ORMLite!F7</f>
         <v>358.4</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
         <v>7</v>
       </c>
@@ -758,42 +804,62 @@
       <c r="D7" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="E7" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B8">
-        <f>1000*1000/D2</f>
+      <c r="B8" s="1">
+        <f t="shared" ref="B8:E9" si="0">1000*1000/D2</f>
         <v>4826.2548262548262</v>
       </c>
-      <c r="C8">
-        <f>1000*1000/E2</f>
+      <c r="C8" s="1">
+        <f t="shared" si="0"/>
         <v>5376.3440860215051</v>
       </c>
-      <c r="D8">
-        <f>1000*1000/F2</f>
+      <c r="D8" s="1">
+        <f t="shared" si="0"/>
+        <v>8635.5785837651129</v>
+      </c>
+      <c r="E8" s="5">
+        <f t="shared" si="0"/>
         <v>6501.9505851755521</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B9">
-        <f>1000*1000/D3</f>
+      <c r="B9" s="1">
+        <f t="shared" si="0"/>
         <v>2223.2103156958647</v>
       </c>
-      <c r="C9">
-        <f>1000*1000/E3</f>
+      <c r="C9" s="1">
+        <f t="shared" si="0"/>
         <v>2190.1007446342533</v>
       </c>
-      <c r="D9">
-        <f>1000*1000/F3</f>
+      <c r="D9" s="1">
+        <f t="shared" si="0"/>
         <v>2790.1785714285716</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E9" s="5"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E10" s="5"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E11" s="5"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E12" s="5"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E13" s="5"/>
+    </row>
+    <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B14" s="3" t="s">
         <v>10</v>
       </c>
@@ -803,18 +869,28 @@
       <c r="D14" s="3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B15">
+      <c r="E14" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" s="1">
         <f>D3/D2</f>
         <v>2.1708494208494211</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="1">
         <f>E3/E2</f>
         <v>2.4548387096774196</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="1">
         <f>F3/F2</f>
+        <v>3.094991364421416</v>
+      </c>
+      <c r="E15" s="5">
+        <f>F3/G2</f>
         <v>2.3302990897269176</v>
       </c>
     </row>
@@ -827,10 +903,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:F7"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -838,10 +914,14 @@
     <col min="1" max="1" width="11.42578125" style="1"/>
     <col min="2" max="2" width="13.42578125" style="1" customWidth="1"/>
     <col min="3" max="3" width="13.5703125" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="11.42578125" style="1"/>
+    <col min="4" max="4" width="14" style="1" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="15" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -855,10 +935,13 @@
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B2" s="1">
         <v>7844</v>
       </c>
@@ -874,8 +957,11 @@
       <c r="F2" s="1">
         <v>163</v>
       </c>
-    </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G2" s="1">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B3" s="1">
         <v>8326</v>
       </c>
@@ -891,8 +977,11 @@
       <c r="F3" s="1">
         <v>150</v>
       </c>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G3" s="1">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B4" s="1">
         <v>8607</v>
       </c>
@@ -908,8 +997,11 @@
       <c r="F4" s="1">
         <v>156</v>
       </c>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G4" s="1">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B5" s="1">
         <v>6275</v>
       </c>
@@ -925,8 +1017,11 @@
       <c r="F5" s="1">
         <v>143</v>
       </c>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G5" s="1">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B6" s="1">
         <v>8511</v>
       </c>
@@ -942,8 +1037,11 @@
       <c r="F6" s="1">
         <v>157</v>
       </c>
-    </row>
-    <row r="7" spans="2:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G6" s="1">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="2">
         <f>AVERAGE(B2:B6)</f>
         <v>7912.6</v>
@@ -963,6 +1061,19 @@
       <c r="F7" s="2">
         <f>AVERAGE(F2:F6)</f>
         <v>153.80000000000001</v>
+      </c>
+      <c r="G7" s="2">
+        <f>AVERAGE(G2:G6)</f>
+        <v>115.8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="1">
+        <f>F7/G7</f>
+        <v>1.3281519861830744</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added performance results for Android 4.0 plus a comparison to 2.3
</commit_message>
<xml_diff>
--- a/DaoGenerator/performance/performance-data.xlsx
+++ b/DaoGenerator/performance/performance-data.xlsx
@@ -4,23 +4,25 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="45" windowWidth="17715" windowHeight="9270" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="45" windowWidth="17715" windowHeight="9270" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="22.8.2011" sheetId="7" r:id="rId1"/>
-    <sheet name="22.8.2011 VS" sheetId="8" r:id="rId2"/>
-    <sheet name="fast cursor" sheetId="6" r:id="rId3"/>
-    <sheet name="Preview3" sheetId="5" r:id="rId4"/>
-    <sheet name="VS" sheetId="2" r:id="rId5"/>
-    <sheet name="greenDAO" sheetId="4" r:id="rId6"/>
-    <sheet name="ORMLite" sheetId="1" r:id="rId7"/>
+    <sheet name="2.3 vs 4.0" sheetId="10" r:id="rId1"/>
+    <sheet name="17.12.2011 Android 4.0.3" sheetId="9" r:id="rId2"/>
+    <sheet name="22.8.2011" sheetId="7" r:id="rId3"/>
+    <sheet name="22.8.2011 VS" sheetId="8" r:id="rId4"/>
+    <sheet name="fast cursor" sheetId="6" r:id="rId5"/>
+    <sheet name="Preview3" sheetId="5" r:id="rId6"/>
+    <sheet name="VS" sheetId="2" r:id="rId7"/>
+    <sheet name="greenDAO" sheetId="4" r:id="rId8"/>
+    <sheet name="ORMLite" sheetId="1" r:id="rId9"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="63">
   <si>
     <t>100x Insert (one-by-one)</t>
   </si>
@@ -189,6 +191,27 @@
   <si>
     <t>Invalid data, too few iterations in preview 3</t>
   </si>
+  <si>
+    <t>Set-up</t>
+  </si>
+  <si>
+    <t>Android 2.3, No Identity Scope</t>
+  </si>
+  <si>
+    <t>Android 2.3, Identity Scope</t>
+  </si>
+  <si>
+    <t>Android 4.0, Identity Scope</t>
+  </si>
+  <si>
+    <t>Android 4.0, No Identity Scope</t>
+  </si>
+  <si>
+    <t>2.3 vs. 4.0, No Identity Scope</t>
+  </si>
+  <si>
+    <t>2.3 vs. 4.0, Identity Scope</t>
+  </si>
 </sst>
 </file>
 
@@ -301,7 +324,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -363,6 +386,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Prozent" xfId="1" builtinId="5"/>
@@ -379,6 +403,184 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="de-DE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>SQL Performance: Android 4.0 vs. 2.3</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Android 4.0 vs. 2.3</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill>
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent3">
+                    <a:lumMod val="50000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent3">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>('2.3 vs 4.0'!$G$2,'2.3 vs 4.0'!$I$2,'2.3 vs 4.0'!$J$2,'2.3 vs 4.0'!$K$2)</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1000x Load</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1000x Insert</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1000x Update</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Delete all (1000)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>('2.3 vs 4.0'!$G$8,'2.3 vs 4.0'!$I$8,'2.3 vs 4.0'!$J$8,'2.3 vs 4.0'!$K$8)</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1.4157706093189966</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.49886104783599089</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.45318181818181819</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.2328767123287672</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="47193088"/>
+        <c:axId val="165012032"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="47193088"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="165012032"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="165012032"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="47193088"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:majorUnit val="0.25"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr>
+          <a:latin typeface="Roboto" pitchFamily="2" charset="0"/>
+          <a:ea typeface="Roboto" pitchFamily="2" charset="0"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="de-DE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="de-DE"/>
@@ -428,7 +630,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'22.8.2011'!$A$23</c:f>
+              <c:f>'17.12.2011 Android 4.0.3'!$A$23</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -466,7 +668,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'22.8.2011'!$G$22:$K$22</c:f>
+              <c:f>'17.12.2011 Android 4.0.3'!$G$22:$K$22</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -489,24 +691,24 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'22.8.2011'!$G$23:$K$23</c:f>
+              <c:f>'17.12.2011 Android 4.0.3'!$G$23:$K$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>12658.227848101265</c:v>
+                  <c:v>17921.146953405016</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>14925.373134328358</c:v>
+                  <c:v>17482.517482517484</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5707.7625570776254</c:v>
+                  <c:v>2847.380410022779</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5015.0451354062188</c:v>
+                  <c:v>2272.727272727273</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>11111.111111111111</c:v>
+                  <c:v>13698.630136986301</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -517,7 +719,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'22.8.2011'!$A$24</c:f>
+              <c:f>'17.12.2011 Android 4.0.3'!$A$24</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -558,7 +760,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'22.8.2011'!$G$22:$K$22</c:f>
+              <c:f>'17.12.2011 Android 4.0.3'!$G$22:$K$22</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -581,24 +783,24 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'22.8.2011'!$G$24:$K$24</c:f>
+              <c:f>'17.12.2011 Android 4.0.3'!$G$24:$K$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>11655.011655011656</c:v>
+                  <c:v>15243.902439024392</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>29761.90476190476</c:v>
+                  <c:v>36764.705882352944</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5574.1360089186173</c:v>
+                  <c:v>2653.9278131634819</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4625.3469010175768</c:v>
+                  <c:v>2383.2221163012391</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>10482.180293501047</c:v>
+                  <c:v>18939.39393939394</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -614,12 +816,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="94580224"/>
-        <c:axId val="88731008"/>
+        <c:axId val="169918464"/>
+        <c:axId val="174206912"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="94580224"/>
+        <c:axId val="169918464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -629,7 +831,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="88731008"/>
+        <c:crossAx val="174206912"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -637,7 +839,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="88731008"/>
+        <c:axId val="174206912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="21000"/>
@@ -650,7 +852,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="94580224"/>
+        <c:crossAx val="169918464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="4000"/>
@@ -669,250 +871,6 @@
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
-      <c:spPr>
-        <a:solidFill>
-          <a:schemeClr val="bg1">
-            <a:lumMod val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </c:spPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="de-DE"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:autoTitleDeleted val="0"/>
-    <c:view3D>
-      <c:rotX val="15"/>
-      <c:rotY val="20"/>
-      <c:rAngAx val="1"/>
-    </c:view3D>
-    <c:floor>
-      <c:thickness val="0"/>
-    </c:floor>
-    <c:sideWall>
-      <c:thickness val="0"/>
-    </c:sideWall>
-    <c:backWall>
-      <c:thickness val="0"/>
-    </c:backWall>
-    <c:plotArea>
-      <c:layout/>
-      <c:bar3DChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'22.8.2011 VS'!$A$8</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>greenDAO</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:gradFill>
-              <a:gsLst>
-                <a:gs pos="0">
-                  <a:srgbClr val="92D050"/>
-                </a:gs>
-                <a:gs pos="50000">
-                  <a:srgbClr val="9CB86E"/>
-                </a:gs>
-                <a:gs pos="100000">
-                  <a:srgbClr val="156B13"/>
-                </a:gs>
-              </a:gsLst>
-              <a:lin ang="5400000" scaled="0"/>
-            </a:gradFill>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>'22.8.2011 VS'!$B$7:$D$7</c:f>
-              <c:strCache>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>Insert/s</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Update/s</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Load/s</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'22.8.2011 VS'!$B$8:$D$8</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>5707.7625570776263</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>5015.0451354062188</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>12658.227848101265</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'22.8.2011 VS'!$A$9</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>ORMLite</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>'22.8.2011 VS'!$B$7:$D$7</c:f>
-              <c:strCache>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>Insert/s</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Update/s</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Load/s</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'22.8.2011 VS'!$B$9:$D$9</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>2223.2103156958647</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2190.1007446342533</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2790.1785714285716</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="150"/>
-        <c:shape val="box"/>
-        <c:axId val="94579712"/>
-        <c:axId val="88733312"/>
-        <c:axId val="0"/>
-      </c:bar3DChart>
-      <c:catAx>
-        <c:axId val="94579712"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="88733312"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="88733312"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln>
-              <a:solidFill>
-                <a:schemeClr val="bg1">
-                  <a:lumMod val="75000"/>
-                </a:schemeClr>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="94579712"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="tr"/>
-      <c:layout>
-        <c:manualLayout>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.2640702099737533"/>
-          <c:y val="0.12260536398467432"/>
-          <c:w val="0.14524883049299578"/>
-          <c:h val="0.12590366152011678"/>
-        </c:manualLayout>
-      </c:layout>
-      <c:overlay val="1"/>
       <c:spPr>
         <a:solidFill>
           <a:schemeClr val="bg1">
@@ -983,7 +941,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'fast cursor'!$A$23</c:f>
+              <c:f>'22.8.2011'!$A$23</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1021,7 +979,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'fast cursor'!$G$22:$K$22</c:f>
+              <c:f>'22.8.2011'!$G$22:$K$22</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -1031,37 +989,37 @@
                   <c:v>Loads/s (2nd time)</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Loads/s (long key)</c:v>
+                  <c:v>Inserts/s</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Loads/s (2nd, long key)</c:v>
+                  <c:v>Updates/s</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Loads/s (Object key)</c:v>
+                  <c:v>Delete (all)/s</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'fast cursor'!$G$23:$K$23</c:f>
+              <c:f>'22.8.2011'!$G$23:$K$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>10683.760683760685</c:v>
+                  <c:v>12658.227848101265</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>15527.950310559005</c:v>
+                  <c:v>14925.373134328358</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>5707.7625570776254</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>5015.0451354062188</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>11111.111111111111</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1072,7 +1030,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'fast cursor'!$A$24</c:f>
+              <c:f>'22.8.2011'!$A$24</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1113,7 +1071,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'fast cursor'!$G$22:$K$22</c:f>
+              <c:f>'22.8.2011'!$G$22:$K$22</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -1123,37 +1081,37 @@
                   <c:v>Loads/s (2nd time)</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Loads/s (long key)</c:v>
+                  <c:v>Inserts/s</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Loads/s (2nd, long key)</c:v>
+                  <c:v>Updates/s</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Loads/s (Object key)</c:v>
+                  <c:v>Delete (all)/s</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'fast cursor'!$G$24:$K$24</c:f>
+              <c:f>'22.8.2011'!$G$24:$K$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>7418.3976261127591</c:v>
+                  <c:v>11655.011655011656</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>24509.803921568629</c:v>
+                  <c:v>29761.90476190476</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9803.9215686274511</c:v>
+                  <c:v>5574.1360089186173</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>25510.204081632652</c:v>
+                  <c:v>4625.3469010175768</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9746.5886939571155</c:v>
+                  <c:v>10482.180293501047</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1169,12 +1127,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="191099392"/>
-        <c:axId val="191987712"/>
+        <c:axId val="165206528"/>
+        <c:axId val="165229056"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="191099392"/>
+        <c:axId val="165206528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1184,7 +1142,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="191987712"/>
+        <c:crossAx val="165229056"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1192,7 +1150,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="191987712"/>
+        <c:axId val="165229056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="21000"/>
@@ -1205,7 +1163,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="191099392"/>
+        <c:crossAx val="165206528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="4000"/>
@@ -1217,8 +1175,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.77282426027681794"/>
-          <c:y val="4.2020563725444993E-2"/>
+          <c:x val="0.72678109480919206"/>
+          <c:y val="9.8900522773982119E-2"/>
           <c:w val="0.21301686210087048"/>
           <c:h val="0.12100651445459654"/>
         </c:manualLayout>
@@ -1274,17 +1232,7 @@
       <c:thickness val="0"/>
     </c:backWall>
     <c:plotArea>
-      <c:layout>
-        <c:manualLayout>
-          <c:layoutTarget val="inner"/>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.11423840769903762"/>
-          <c:y val="5.1400554097404488E-2"/>
-          <c:w val="0.84955314960629913"/>
-          <c:h val="0.77175014581510648"/>
-        </c:manualLayout>
-      </c:layout>
+      <c:layout/>
       <c:bar3DChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
@@ -1294,85 +1242,63 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Preview3!$A$23</c:f>
+              <c:f>'22.8.2011 VS'!$A$8</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Without Identity Scope</c:v>
+                  <c:v>greenDAO</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:gradFill flip="none" rotWithShape="1">
+            <a:gradFill>
               <a:gsLst>
                 <a:gs pos="0">
-                  <a:srgbClr val="92D050">
-                    <a:shade val="30000"/>
-                    <a:satMod val="115000"/>
-                  </a:srgbClr>
+                  <a:srgbClr val="92D050"/>
                 </a:gs>
                 <a:gs pos="50000">
-                  <a:srgbClr val="92D050">
-                    <a:shade val="67500"/>
-                    <a:satMod val="115000"/>
-                  </a:srgbClr>
+                  <a:srgbClr val="9CB86E"/>
                 </a:gs>
                 <a:gs pos="100000">
-                  <a:srgbClr val="92D050">
-                    <a:shade val="100000"/>
-                    <a:satMod val="115000"/>
-                  </a:srgbClr>
+                  <a:srgbClr val="156B13"/>
                 </a:gs>
               </a:gsLst>
-              <a:lin ang="2700000" scaled="1"/>
-              <a:tileRect/>
+              <a:lin ang="5400000" scaled="0"/>
             </a:gradFill>
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Preview3!$G$22:$K$22</c:f>
+              <c:f>'22.8.2011 VS'!$B$7:$D$7</c:f>
               <c:strCache>
-                <c:ptCount val="5"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>Loads/s</c:v>
+                  <c:v>Insert/s</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Loads/s (2nd time)</c:v>
+                  <c:v>Update/s</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Inserts/s</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Updates/s</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Delete (all)/s</c:v>
+                  <c:v>Load/s</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Preview3!$G$23:$K$23</c:f>
+              <c:f>'22.8.2011 VS'!$B$8:$D$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>8103.7277147487839</c:v>
+                  <c:v>5707.7625570776263</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>11520.737327188941</c:v>
+                  <c:v>5015.0451354062188</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5567.9287305122498</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>5422.9934924078088</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>15384.615384615385</c:v>
+                  <c:v>12658.227848101265</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1383,88 +1309,47 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Preview3!$A$24</c:f>
+              <c:f>'22.8.2011 VS'!$A$9</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>With Identity Scope</c:v>
+                  <c:v>ORMLite</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:spPr>
-            <a:gradFill flip="none" rotWithShape="1">
-              <a:gsLst>
-                <a:gs pos="0">
-                  <a:schemeClr val="accent3">
-                    <a:lumMod val="75000"/>
-                    <a:shade val="30000"/>
-                    <a:satMod val="115000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="50000">
-                  <a:schemeClr val="accent3">
-                    <a:lumMod val="75000"/>
-                    <a:shade val="67500"/>
-                    <a:satMod val="115000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="100000">
-                  <a:schemeClr val="accent3">
-                    <a:lumMod val="75000"/>
-                    <a:shade val="100000"/>
-                    <a:satMod val="115000"/>
-                  </a:schemeClr>
-                </a:gs>
-              </a:gsLst>
-              <a:lin ang="2700000" scaled="1"/>
-              <a:tileRect/>
-            </a:gradFill>
-          </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Preview3!$G$22:$K$22</c:f>
+              <c:f>'22.8.2011 VS'!$B$7:$D$7</c:f>
               <c:strCache>
-                <c:ptCount val="5"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>Loads/s</c:v>
+                  <c:v>Insert/s</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Loads/s (2nd time)</c:v>
+                  <c:v>Update/s</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Inserts/s</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Updates/s</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Delete (all)/s</c:v>
+                  <c:v>Load/s</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Preview3!$G$24:$K$24</c:f>
+              <c:f>'22.8.2011 VS'!$B$9:$D$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>5144.032921810699</c:v>
+                  <c:v>2223.2103156958647</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>21008.403361344539</c:v>
+                  <c:v>2190.1007446342533</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4314.0638481449523</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4990.0199600798396</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>13774.104683195594</c:v>
+                  <c:v>2790.1785714285716</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1480,22 +1365,21 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="191101440"/>
-        <c:axId val="191990016"/>
+        <c:axId val="166469120"/>
+        <c:axId val="165231360"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="191101440"/>
+        <c:axId val="166469120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="191990016"/>
+        <c:crossAx val="165231360"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1503,38 +1387,45 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="191990016"/>
+        <c:axId val="165231360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="21000"/>
-          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
-        <c:majorGridlines/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="bg1">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="191101440"/>
+        <c:crossAx val="166469120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
-        <c:majorUnit val="4000"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="r"/>
+      <c:legendPos val="tr"/>
       <c:layout>
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.72678109480919206"/>
-          <c:y val="9.8900522773982119E-2"/>
-          <c:w val="0.21301686210087048"/>
-          <c:h val="0.12100651445459654"/>
+          <c:x val="0.2640702099737533"/>
+          <c:y val="0.12260536398467432"/>
+          <c:w val="0.14524883049299578"/>
+          <c:h val="0.12590366152011678"/>
         </c:manualLayout>
       </c:layout>
-      <c:overlay val="0"/>
+      <c:overlay val="1"/>
       <c:spPr>
         <a:solidFill>
           <a:schemeClr val="bg1">
@@ -1585,6 +1476,628 @@
       <c:thickness val="0"/>
     </c:backWall>
     <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.11423840769903762"/>
+          <c:y val="5.1400554097404488E-2"/>
+          <c:w val="0.84955314960629913"/>
+          <c:h val="0.77175014581510648"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:bar3DChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'fast cursor'!$A$23</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Without Identity Scope</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill flip="none" rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:srgbClr val="92D050">
+                    <a:shade val="30000"/>
+                    <a:satMod val="115000"/>
+                  </a:srgbClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:srgbClr val="92D050">
+                    <a:shade val="67500"/>
+                    <a:satMod val="115000"/>
+                  </a:srgbClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:srgbClr val="92D050">
+                    <a:shade val="100000"/>
+                    <a:satMod val="115000"/>
+                  </a:srgbClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="2700000" scaled="1"/>
+              <a:tileRect/>
+            </a:gradFill>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'fast cursor'!$G$22:$K$22</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Loads/s</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Loads/s (2nd time)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Loads/s (long key)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Loads/s (2nd, long key)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Loads/s (Object key)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'fast cursor'!$G$23:$K$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>10683.760683760685</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15527.950310559005</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'fast cursor'!$A$24</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>With Identity Scope</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill flip="none" rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent3">
+                    <a:lumMod val="75000"/>
+                    <a:shade val="30000"/>
+                    <a:satMod val="115000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent3">
+                    <a:lumMod val="75000"/>
+                    <a:shade val="67500"/>
+                    <a:satMod val="115000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent3">
+                    <a:lumMod val="75000"/>
+                    <a:shade val="100000"/>
+                    <a:satMod val="115000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="2700000" scaled="1"/>
+              <a:tileRect/>
+            </a:gradFill>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'fast cursor'!$G$22:$K$22</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Loads/s</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Loads/s (2nd time)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Loads/s (long key)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Loads/s (2nd, long key)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Loads/s (Object key)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'fast cursor'!$G$24:$K$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>7418.3976261127591</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>24509.803921568629</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9803.9215686274511</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>25510.204081632652</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9746.5886939571155</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:shape val="box"/>
+        <c:axId val="169772544"/>
+        <c:axId val="167912576"/>
+        <c:axId val="0"/>
+      </c:bar3DChart>
+      <c:catAx>
+        <c:axId val="169772544"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="167912576"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="167912576"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="21000"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="169772544"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:majorUnit val="4000"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.77282426027681794"/>
+          <c:y val="4.2020563725444993E-2"/>
+          <c:w val="0.21301686210087048"/>
+          <c:h val="0.12100651445459654"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:solidFill>
+          <a:schemeClr val="bg1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </c:spPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="de-DE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:view3D>
+      <c:rotX val="15"/>
+      <c:rotY val="20"/>
+      <c:rAngAx val="1"/>
+    </c:view3D>
+    <c:floor>
+      <c:thickness val="0"/>
+    </c:floor>
+    <c:sideWall>
+      <c:thickness val="0"/>
+    </c:sideWall>
+    <c:backWall>
+      <c:thickness val="0"/>
+    </c:backWall>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.11423840769903762"/>
+          <c:y val="5.1400554097404488E-2"/>
+          <c:w val="0.84955314960629913"/>
+          <c:h val="0.77175014581510648"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:bar3DChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Preview3!$A$23</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Without Identity Scope</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill flip="none" rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:srgbClr val="92D050">
+                    <a:shade val="30000"/>
+                    <a:satMod val="115000"/>
+                  </a:srgbClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:srgbClr val="92D050">
+                    <a:shade val="67500"/>
+                    <a:satMod val="115000"/>
+                  </a:srgbClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:srgbClr val="92D050">
+                    <a:shade val="100000"/>
+                    <a:satMod val="115000"/>
+                  </a:srgbClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="2700000" scaled="1"/>
+              <a:tileRect/>
+            </a:gradFill>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Preview3!$G$22:$K$22</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Loads/s</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Loads/s (2nd time)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Inserts/s</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Updates/s</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Delete (all)/s</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Preview3!$G$23:$K$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>8103.7277147487839</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11520.737327188941</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5567.9287305122498</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5422.9934924078088</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>15384.615384615385</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Preview3!$A$24</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>With Identity Scope</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill flip="none" rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent3">
+                    <a:lumMod val="75000"/>
+                    <a:shade val="30000"/>
+                    <a:satMod val="115000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent3">
+                    <a:lumMod val="75000"/>
+                    <a:shade val="67500"/>
+                    <a:satMod val="115000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent3">
+                    <a:lumMod val="75000"/>
+                    <a:shade val="100000"/>
+                    <a:satMod val="115000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="2700000" scaled="1"/>
+              <a:tileRect/>
+            </a:gradFill>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Preview3!$G$22:$K$22</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Loads/s</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Loads/s (2nd time)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Inserts/s</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Updates/s</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Delete (all)/s</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Preview3!$G$24:$K$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>5144.032921810699</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>21008.403361344539</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4314.0638481449523</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4990.0199600798396</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>13774.104683195594</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:shape val="box"/>
+        <c:axId val="166468608"/>
+        <c:axId val="167914880"/>
+        <c:axId val="0"/>
+      </c:bar3DChart>
+      <c:catAx>
+        <c:axId val="166468608"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="167914880"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="167914880"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="21000"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="166468608"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:majorUnit val="4000"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.72678109480919206"/>
+          <c:y val="9.8900522773982119E-2"/>
+          <c:w val="0.21301686210087048"/>
+          <c:h val="0.12100651445459654"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:solidFill>
+          <a:schemeClr val="bg1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </c:spPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="de-DE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:view3D>
+      <c:rotX val="15"/>
+      <c:rotY val="20"/>
+      <c:rAngAx val="1"/>
+    </c:view3D>
+    <c:floor>
+      <c:thickness val="0"/>
+    </c:floor>
+    <c:sideWall>
+      <c:thickness val="0"/>
+    </c:sideWall>
+    <c:backWall>
+      <c:thickness val="0"/>
+    </c:backWall>
+    <c:plotArea>
       <c:layout/>
       <c:bar3DChart>
         <c:barDir val="col"/>
@@ -1718,12 +2231,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="192114176"/>
-        <c:axId val="191992320"/>
+        <c:axId val="165207040"/>
+        <c:axId val="167917184"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="192114176"/>
+        <c:axId val="165207040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1732,7 +2245,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="191992320"/>
+        <c:crossAx val="167917184"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1740,7 +2253,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="191992320"/>
+        <c:axId val="167917184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1761,7 +2274,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="192114176"/>
+        <c:crossAx val="165207040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1803,6 +2316,41 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>314324</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>119062</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Diagramm 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>723899</xdr:colOff>
       <xdr:row>34</xdr:row>
@@ -1836,7 +2384,44 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>723899</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>166686</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>476249</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Diagramm 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -1873,7 +2458,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -1910,7 +2495,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -1945,7 +2530,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -2267,10 +2852,1229 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K9"/>
+  <sheetViews>
+    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M25" sqref="M25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+    </row>
+    <row r="2" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B3">
+        <v>841.2</v>
+      </c>
+      <c r="C3">
+        <v>834.6</v>
+      </c>
+      <c r="D3">
+        <v>8567.6</v>
+      </c>
+      <c r="E3">
+        <v>8302.4</v>
+      </c>
+      <c r="F3">
+        <v>6943.8</v>
+      </c>
+      <c r="G3">
+        <v>55.8</v>
+      </c>
+      <c r="H3">
+        <v>57.2</v>
+      </c>
+      <c r="I3">
+        <v>351.2</v>
+      </c>
+      <c r="J3">
+        <v>440</v>
+      </c>
+      <c r="K3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B4" s="14">
+        <v>940.8</v>
+      </c>
+      <c r="C4" s="14">
+        <v>9.6</v>
+      </c>
+      <c r="D4" s="14">
+        <v>8684.6</v>
+      </c>
+      <c r="E4" s="14">
+        <v>6822.8</v>
+      </c>
+      <c r="F4" s="14">
+        <v>8892.4</v>
+      </c>
+      <c r="G4" s="1">
+        <v>65.599999999999994</v>
+      </c>
+      <c r="H4" s="1">
+        <v>27.2</v>
+      </c>
+      <c r="I4" s="1">
+        <v>376.8</v>
+      </c>
+      <c r="J4" s="1">
+        <v>419.6</v>
+      </c>
+      <c r="K4" s="1">
+        <v>52.8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B5" s="14">
+        <v>574.6</v>
+      </c>
+      <c r="C5" s="14">
+        <v>563</v>
+      </c>
+      <c r="D5" s="14">
+        <v>8519</v>
+      </c>
+      <c r="E5" s="14">
+        <v>8142.8</v>
+      </c>
+      <c r="F5" s="14">
+        <v>7633.2</v>
+      </c>
+      <c r="G5" s="1">
+        <v>79</v>
+      </c>
+      <c r="H5" s="1">
+        <v>67</v>
+      </c>
+      <c r="I5" s="1">
+        <v>175.2</v>
+      </c>
+      <c r="J5" s="1">
+        <v>199.4</v>
+      </c>
+      <c r="K5" s="1">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>58</v>
+      </c>
+      <c r="B6" s="14">
+        <v>633.6</v>
+      </c>
+      <c r="C6" s="14">
+        <v>7.6</v>
+      </c>
+      <c r="D6" s="14">
+        <v>7833.6</v>
+      </c>
+      <c r="E6" s="14">
+        <v>7690.8</v>
+      </c>
+      <c r="F6" s="14">
+        <v>7480.8</v>
+      </c>
+      <c r="G6" s="1">
+        <v>85.8</v>
+      </c>
+      <c r="H6" s="1">
+        <v>33.6</v>
+      </c>
+      <c r="I6" s="1">
+        <v>179.4</v>
+      </c>
+      <c r="J6" s="1">
+        <v>216.2</v>
+      </c>
+      <c r="K6" s="1">
+        <v>95.4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B7" s="14"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B8" s="9">
+        <f>B5/B3</f>
+        <v>0.68307180218735142</v>
+      </c>
+      <c r="C8" s="9">
+        <f>C5/C3</f>
+        <v>0.67457464653726329</v>
+      </c>
+      <c r="D8" s="9">
+        <f>D5/D3</f>
+        <v>0.9943274662682664</v>
+      </c>
+      <c r="E8" s="9">
+        <f>E5/E3</f>
+        <v>0.98077664289843902</v>
+      </c>
+      <c r="F8" s="9">
+        <f>F5/F3</f>
+        <v>1.0992828134450876</v>
+      </c>
+      <c r="G8" s="9">
+        <f>G5/G3</f>
+        <v>1.4157706093189966</v>
+      </c>
+      <c r="H8" s="9">
+        <f>H5/H3</f>
+        <v>1.1713286713286712</v>
+      </c>
+      <c r="I8" s="9">
+        <f>I5/I3</f>
+        <v>0.49886104783599089</v>
+      </c>
+      <c r="J8" s="9">
+        <f>J5/J3</f>
+        <v>0.45318181818181819</v>
+      </c>
+      <c r="K8" s="9">
+        <f>K5/K3</f>
+        <v>1.2328767123287672</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>62</v>
+      </c>
+      <c r="B9" s="9">
+        <f>B6/B4</f>
+        <v>0.67346938775510212</v>
+      </c>
+      <c r="C9" s="9">
+        <f t="shared" ref="C9:K9" si="0">C6/C4</f>
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="D9" s="9">
+        <f t="shared" si="0"/>
+        <v>0.90201045528867185</v>
+      </c>
+      <c r="E9" s="9">
+        <f t="shared" si="0"/>
+        <v>1.1272204959840535</v>
+      </c>
+      <c r="F9" s="9">
+        <f t="shared" si="0"/>
+        <v>0.84125770320723314</v>
+      </c>
+      <c r="G9" s="9">
+        <f t="shared" si="0"/>
+        <v>1.3079268292682928</v>
+      </c>
+      <c r="H9" s="9">
+        <f t="shared" si="0"/>
+        <v>1.2352941176470589</v>
+      </c>
+      <c r="I9" s="9">
+        <f t="shared" si="0"/>
+        <v>0.47611464968152867</v>
+      </c>
+      <c r="J9" s="9">
+        <f t="shared" si="0"/>
+        <v>0.51525262154432783</v>
+      </c>
+      <c r="K9" s="9">
+        <f t="shared" si="0"/>
+        <v>1.8068181818181821</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="G1:K1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K30"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="M39" sqref="M39"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="20.5703125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="14" style="1" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="15" style="1" customWidth="1"/>
+    <col min="8" max="8" width="20.5703125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="14.7109375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="14" style="1" customWidth="1"/>
+    <col min="11" max="11" width="15.42578125" style="1" customWidth="1"/>
+    <col min="12" max="16384" width="11.42578125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+    </row>
+    <row r="2" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="19"/>
+      <c r="B2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="19"/>
+      <c r="B3" s="14">
+        <v>969</v>
+      </c>
+      <c r="C3" s="14">
+        <v>896</v>
+      </c>
+      <c r="D3" s="14">
+        <v>10137</v>
+      </c>
+      <c r="E3" s="14">
+        <v>7467</v>
+      </c>
+      <c r="F3" s="14">
+        <v>7866</v>
+      </c>
+      <c r="G3" s="1">
+        <v>55</v>
+      </c>
+      <c r="H3" s="1">
+        <v>56</v>
+      </c>
+      <c r="I3" s="1">
+        <v>422</v>
+      </c>
+      <c r="J3" s="1">
+        <v>450</v>
+      </c>
+      <c r="K3" s="1">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="19"/>
+      <c r="B4" s="14">
+        <v>813</v>
+      </c>
+      <c r="C4" s="14">
+        <v>828</v>
+      </c>
+      <c r="D4" s="14">
+        <v>8659</v>
+      </c>
+      <c r="E4" s="14">
+        <v>6625</v>
+      </c>
+      <c r="F4" s="14">
+        <v>5811</v>
+      </c>
+      <c r="G4" s="1">
+        <v>56</v>
+      </c>
+      <c r="H4" s="1">
+        <v>55</v>
+      </c>
+      <c r="I4" s="1">
+        <v>320</v>
+      </c>
+      <c r="J4" s="1">
+        <v>412</v>
+      </c>
+      <c r="K4" s="1">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="19"/>
+      <c r="B5" s="14">
+        <v>816</v>
+      </c>
+      <c r="C5" s="14">
+        <v>825</v>
+      </c>
+      <c r="D5" s="14">
+        <v>8856</v>
+      </c>
+      <c r="E5" s="14">
+        <v>8657</v>
+      </c>
+      <c r="F5" s="14">
+        <v>8236</v>
+      </c>
+      <c r="G5" s="1">
+        <v>56</v>
+      </c>
+      <c r="H5" s="1">
+        <v>56</v>
+      </c>
+      <c r="I5" s="1">
+        <v>356</v>
+      </c>
+      <c r="J5" s="1">
+        <v>377</v>
+      </c>
+      <c r="K5" s="1">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="19"/>
+      <c r="B6" s="14">
+        <v>805</v>
+      </c>
+      <c r="C6" s="14">
+        <v>814</v>
+      </c>
+      <c r="D6" s="14">
+        <v>7793</v>
+      </c>
+      <c r="E6" s="14">
+        <v>10340</v>
+      </c>
+      <c r="F6" s="14">
+        <v>6145</v>
+      </c>
+      <c r="G6" s="1">
+        <v>56</v>
+      </c>
+      <c r="H6" s="1">
+        <v>55</v>
+      </c>
+      <c r="I6" s="1">
+        <v>329</v>
+      </c>
+      <c r="J6" s="1">
+        <v>489</v>
+      </c>
+      <c r="K6" s="1">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="19"/>
+      <c r="B7" s="14">
+        <v>803</v>
+      </c>
+      <c r="C7" s="14">
+        <v>810</v>
+      </c>
+      <c r="D7" s="14">
+        <v>7393</v>
+      </c>
+      <c r="E7" s="14">
+        <v>8423</v>
+      </c>
+      <c r="F7" s="14">
+        <v>6661</v>
+      </c>
+      <c r="G7" s="1">
+        <v>56</v>
+      </c>
+      <c r="H7" s="1">
+        <v>64</v>
+      </c>
+      <c r="I7" s="1">
+        <v>329</v>
+      </c>
+      <c r="J7" s="1">
+        <v>472</v>
+      </c>
+      <c r="K7" s="1">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="19"/>
+      <c r="B8" s="2">
+        <f t="shared" ref="B8:K8" si="0">AVERAGE(B3:B7)</f>
+        <v>841.2</v>
+      </c>
+      <c r="C8" s="2">
+        <f t="shared" si="0"/>
+        <v>834.6</v>
+      </c>
+      <c r="D8" s="2">
+        <f t="shared" si="0"/>
+        <v>8567.6</v>
+      </c>
+      <c r="E8" s="2">
+        <f t="shared" si="0"/>
+        <v>8302.4</v>
+      </c>
+      <c r="F8" s="2">
+        <f t="shared" si="0"/>
+        <v>6943.8</v>
+      </c>
+      <c r="G8" s="2">
+        <f t="shared" si="0"/>
+        <v>55.8</v>
+      </c>
+      <c r="H8" s="2">
+        <f t="shared" si="0"/>
+        <v>57.2</v>
+      </c>
+      <c r="I8" s="2">
+        <f t="shared" si="0"/>
+        <v>351.2</v>
+      </c>
+      <c r="J8" s="2">
+        <f t="shared" si="0"/>
+        <v>440</v>
+      </c>
+      <c r="K8" s="2">
+        <f t="shared" si="0"/>
+        <v>73</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B9" s="14"/>
+      <c r="C9" s="14"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="20"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="H10" s="16"/>
+      <c r="I10" s="16"/>
+      <c r="J10" s="16"/>
+      <c r="K10" s="16"/>
+    </row>
+    <row r="11" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="19"/>
+      <c r="B11" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="K11" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="19"/>
+      <c r="B12" s="14">
+        <v>1125</v>
+      </c>
+      <c r="C12" s="14">
+        <v>11</v>
+      </c>
+      <c r="D12" s="14">
+        <v>8675</v>
+      </c>
+      <c r="E12" s="14">
+        <v>8494</v>
+      </c>
+      <c r="F12" s="14">
+        <v>8059</v>
+      </c>
+      <c r="G12" s="1">
+        <v>64</v>
+      </c>
+      <c r="H12" s="1">
+        <v>27</v>
+      </c>
+      <c r="I12" s="1">
+        <v>462</v>
+      </c>
+      <c r="J12" s="1">
+        <v>407</v>
+      </c>
+      <c r="K12" s="1">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="19"/>
+      <c r="B13" s="14">
+        <v>884</v>
+      </c>
+      <c r="C13" s="14">
+        <v>10</v>
+      </c>
+      <c r="D13" s="14">
+        <v>8424</v>
+      </c>
+      <c r="E13" s="14">
+        <v>6071</v>
+      </c>
+      <c r="F13" s="14">
+        <v>7742</v>
+      </c>
+      <c r="G13" s="1">
+        <v>64</v>
+      </c>
+      <c r="H13" s="1">
+        <v>27</v>
+      </c>
+      <c r="I13" s="1">
+        <v>358</v>
+      </c>
+      <c r="J13" s="1">
+        <v>468</v>
+      </c>
+      <c r="K13" s="1">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="19"/>
+      <c r="B14" s="14">
+        <v>930</v>
+      </c>
+      <c r="C14" s="14">
+        <v>10</v>
+      </c>
+      <c r="D14" s="14">
+        <v>9301</v>
+      </c>
+      <c r="E14" s="14">
+        <v>5355</v>
+      </c>
+      <c r="F14" s="14">
+        <v>9759</v>
+      </c>
+      <c r="G14" s="1">
+        <v>65</v>
+      </c>
+      <c r="H14" s="1">
+        <v>27</v>
+      </c>
+      <c r="I14" s="1">
+        <v>330</v>
+      </c>
+      <c r="J14" s="1">
+        <v>411</v>
+      </c>
+      <c r="K14" s="1">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="19"/>
+      <c r="B15" s="14">
+        <v>884</v>
+      </c>
+      <c r="C15" s="14">
+        <v>9</v>
+      </c>
+      <c r="D15" s="14">
+        <v>9785</v>
+      </c>
+      <c r="E15" s="14">
+        <v>7125</v>
+      </c>
+      <c r="F15" s="14">
+        <v>10689</v>
+      </c>
+      <c r="G15" s="1">
+        <v>65</v>
+      </c>
+      <c r="H15" s="1">
+        <v>27</v>
+      </c>
+      <c r="I15" s="1">
+        <v>379</v>
+      </c>
+      <c r="J15" s="1">
+        <v>437</v>
+      </c>
+      <c r="K15" s="1">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="19"/>
+      <c r="B16" s="14">
+        <v>881</v>
+      </c>
+      <c r="C16" s="14">
+        <v>8</v>
+      </c>
+      <c r="D16" s="14">
+        <v>7238</v>
+      </c>
+      <c r="E16" s="14">
+        <v>7069</v>
+      </c>
+      <c r="F16" s="14">
+        <v>8213</v>
+      </c>
+      <c r="G16" s="1">
+        <v>70</v>
+      </c>
+      <c r="H16" s="1">
+        <v>28</v>
+      </c>
+      <c r="I16" s="1">
+        <v>355</v>
+      </c>
+      <c r="J16" s="1">
+        <v>375</v>
+      </c>
+      <c r="K16" s="1">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="19"/>
+      <c r="B17" s="2">
+        <f t="shared" ref="B17:K17" si="1">AVERAGE(B12:B16)</f>
+        <v>940.8</v>
+      </c>
+      <c r="C17" s="2">
+        <f t="shared" si="1"/>
+        <v>9.6</v>
+      </c>
+      <c r="D17" s="2">
+        <f t="shared" si="1"/>
+        <v>8684.6</v>
+      </c>
+      <c r="E17" s="2">
+        <f t="shared" si="1"/>
+        <v>6822.8</v>
+      </c>
+      <c r="F17" s="2">
+        <f t="shared" si="1"/>
+        <v>8892.4</v>
+      </c>
+      <c r="G17" s="2">
+        <f t="shared" si="1"/>
+        <v>65.599999999999994</v>
+      </c>
+      <c r="H17" s="2">
+        <f t="shared" si="1"/>
+        <v>27.2</v>
+      </c>
+      <c r="I17" s="2">
+        <f t="shared" si="1"/>
+        <v>376.8</v>
+      </c>
+      <c r="J17" s="2">
+        <f t="shared" si="1"/>
+        <v>419.6</v>
+      </c>
+      <c r="K17" s="2">
+        <f t="shared" si="1"/>
+        <v>52.8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="2"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="2"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="2"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2"/>
+      <c r="K20" s="2"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="7"/>
+      <c r="B21" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="C21" s="15"/>
+      <c r="D21" s="15"/>
+      <c r="E21" s="15"/>
+      <c r="F21" s="15"/>
+      <c r="G21" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="H21" s="16"/>
+      <c r="I21" s="16"/>
+      <c r="J21" s="16"/>
+      <c r="K21" s="16"/>
+    </row>
+    <row r="22" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="7"/>
+      <c r="B22" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="H22" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="I22" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="J22" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="K22" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B23" s="14">
+        <f>1000/B8*1000</f>
+        <v>1188.7779362815024</v>
+      </c>
+      <c r="C23" s="14">
+        <f>1000/C8*1000</f>
+        <v>1198.1787682722263</v>
+      </c>
+      <c r="D23" s="14">
+        <f>1000/D8*100</f>
+        <v>11.671880106447546</v>
+      </c>
+      <c r="E23" s="14">
+        <f>1000/E8*100</f>
+        <v>12.044709963384083</v>
+      </c>
+      <c r="F23" s="14">
+        <f>1000/F8*100</f>
+        <v>14.401336444022006</v>
+      </c>
+      <c r="G23" s="1">
+        <f>1000/G8*1000</f>
+        <v>17921.146953405016</v>
+      </c>
+      <c r="H23" s="1">
+        <f>1000/H8*1000</f>
+        <v>17482.517482517484</v>
+      </c>
+      <c r="I23" s="1">
+        <f>1000/I8*1000</f>
+        <v>2847.380410022779</v>
+      </c>
+      <c r="J23" s="1">
+        <f>1000/J8*1000</f>
+        <v>2272.727272727273</v>
+      </c>
+      <c r="K23" s="1">
+        <f>1000/K8*1000</f>
+        <v>13698.630136986301</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B24" s="1">
+        <f>1000/B17*1000</f>
+        <v>1062.9251700680272</v>
+      </c>
+      <c r="C24" s="1">
+        <f>1000/C17*1000</f>
+        <v>104166.66666666667</v>
+      </c>
+      <c r="D24" s="14">
+        <f>1000/D17*100</f>
+        <v>11.514635101213642</v>
+      </c>
+      <c r="E24" s="14">
+        <f>1000/E17*100</f>
+        <v>14.656739168669755</v>
+      </c>
+      <c r="F24" s="14">
+        <f>1000/F17*100</f>
+        <v>11.245558004588188</v>
+      </c>
+      <c r="G24" s="1">
+        <f>1000/G17*1000</f>
+        <v>15243.902439024392</v>
+      </c>
+      <c r="H24" s="1">
+        <f>1000/H17*1000</f>
+        <v>36764.705882352944</v>
+      </c>
+      <c r="I24" s="1">
+        <f>1000/I17*1000</f>
+        <v>2653.9278131634819</v>
+      </c>
+      <c r="J24" s="1">
+        <f>1000/J17*1000</f>
+        <v>2383.2221163012391</v>
+      </c>
+      <c r="K24" s="1">
+        <f>1000/K17*1000</f>
+        <v>18939.39393939394</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B25" s="9">
+        <f>B24/B23</f>
+        <v>0.89413265306122469</v>
+      </c>
+      <c r="C25" s="9">
+        <f t="shared" ref="C25:K25" si="2">C24/C23</f>
+        <v>86.9375</v>
+      </c>
+      <c r="D25" s="9">
+        <f t="shared" si="2"/>
+        <v>0.98652787693158006</v>
+      </c>
+      <c r="E25" s="9">
+        <f t="shared" si="2"/>
+        <v>1.2168611127396376</v>
+      </c>
+      <c r="F25" s="9">
+        <f t="shared" si="2"/>
+        <v>0.78086905672259466</v>
+      </c>
+      <c r="G25" s="9">
+        <f t="shared" si="2"/>
+        <v>0.85060975609756118</v>
+      </c>
+      <c r="H25" s="9">
+        <f t="shared" si="2"/>
+        <v>2.1029411764705883</v>
+      </c>
+      <c r="I25" s="9">
+        <f t="shared" si="2"/>
+        <v>0.93205944798301488</v>
+      </c>
+      <c r="J25" s="9">
+        <f t="shared" si="2"/>
+        <v>1.0486177311725451</v>
+      </c>
+      <c r="K25" s="9">
+        <f t="shared" si="2"/>
+        <v>1.3825757575757576</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B27" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="C27" s="17"/>
+      <c r="D27" s="17"/>
+      <c r="E27" s="17"/>
+      <c r="F27" s="17"/>
+      <c r="G27" s="17"/>
+      <c r="H27" s="17"/>
+      <c r="I27" s="17"/>
+      <c r="J27" s="17"/>
+      <c r="K27" s="17"/>
+    </row>
+    <row r="28" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B28" s="9">
+        <f>B23/Preview3!B23</f>
+        <v>0.81431288635282917</v>
+      </c>
+      <c r="C28" s="9">
+        <f>C23/Preview3!C23</f>
+        <v>0.87107596453390845</v>
+      </c>
+      <c r="D28" s="13">
+        <f>D23/Preview3!D23</f>
+        <v>0.98463980577991495</v>
+      </c>
+      <c r="E28" s="13">
+        <f>E23/Preview3!E23</f>
+        <v>1.3644247446521489</v>
+      </c>
+      <c r="F28" s="13">
+        <f>F23/Preview3!F23</f>
+        <v>0.87934560327198374</v>
+      </c>
+      <c r="G28" s="9">
+        <f>G23/Preview3!G23</f>
+        <v>2.2114695340501789</v>
+      </c>
+      <c r="H28" s="9">
+        <f>H23/Preview3!H23</f>
+        <v>1.5174825174825175</v>
+      </c>
+      <c r="I28" s="9">
+        <f>I23/Preview3!I23</f>
+        <v>0.5113895216400911</v>
+      </c>
+      <c r="J28" s="9">
+        <f>J23/Preview3!J23</f>
+        <v>0.41909090909090918</v>
+      </c>
+      <c r="K28" s="9">
+        <f>K23/Preview3!K23</f>
+        <v>0.8904109589041096</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B29" s="9">
+        <f>B24/Preview3!B24</f>
+        <v>0.70918367346938782</v>
+      </c>
+      <c r="C29" s="9">
+        <f>C24/Preview3!C24</f>
+        <v>0.85416666666666663</v>
+      </c>
+      <c r="D29" s="13">
+        <f>D24/Preview3!D24</f>
+        <v>0.72035557193192556</v>
+      </c>
+      <c r="E29" s="13">
+        <f>E24/Preview3!E24</f>
+        <v>1.0511813331769948</v>
+      </c>
+      <c r="F29" s="13">
+        <f>F24/Preview3!F24</f>
+        <v>0.59219108452161395</v>
+      </c>
+      <c r="G29" s="9">
+        <f>G24/Preview3!G24</f>
+        <v>2.9634146341463423</v>
+      </c>
+      <c r="H29" s="9">
+        <f>H24/Preview3!H24</f>
+        <v>1.75</v>
+      </c>
+      <c r="I29" s="9">
+        <f>I24/Preview3!I24</f>
+        <v>0.61518046709129515</v>
+      </c>
+      <c r="J29" s="9">
+        <f>J24/Preview3!J24</f>
+        <v>0.47759771210676838</v>
+      </c>
+      <c r="K29" s="9">
+        <f>K24/Preview3!K24</f>
+        <v>1.375</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D30" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="E30" s="18"/>
+      <c r="F30" s="18"/>
+    </row>
+  </sheetData>
+  <mergeCells count="10">
+    <mergeCell ref="B21:F21"/>
+    <mergeCell ref="G21:K21"/>
+    <mergeCell ref="B27:K27"/>
+    <mergeCell ref="D30:F30"/>
+    <mergeCell ref="A1:A8"/>
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="G1:K1"/>
+    <mergeCell ref="A10:A17"/>
+    <mergeCell ref="B10:F10"/>
+    <mergeCell ref="G10:K10"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K30"/>
+  <sheetViews>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17:K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3167,7 +4971,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G15"/>
   <sheetViews>
@@ -3278,7 +5082,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="1">
-        <f t="shared" ref="B8:E9" si="0">1000*1000/D2</f>
+        <f t="shared" ref="B8:D9" si="0">1000*1000/D2</f>
         <v>5707.7625570776263</v>
       </c>
       <c r="C8" s="1">
@@ -3358,11 +5162,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
@@ -4020,7 +5824,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K25"/>
   <sheetViews>
@@ -4813,7 +6617,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G15"/>
   <sheetViews>
@@ -5014,7 +6818,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H10"/>
   <sheetViews>
@@ -5227,7 +7031,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:F7"/>
   <sheetViews>

</xml_diff>

<commit_message>
updated ormlite libs to 4.34-SNAPSHOT and performance test against it
</commit_message>
<xml_diff>
--- a/DaoGenerator/performance/performance-data.xlsx
+++ b/DaoGenerator/performance/performance-data.xlsx
@@ -4,25 +4,26 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="45" windowWidth="17715" windowHeight="9270" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="45" windowWidth="17715" windowHeight="9270" tabRatio="734"/>
   </bookViews>
   <sheets>
-    <sheet name="2.3 vs 4.0" sheetId="10" r:id="rId1"/>
-    <sheet name="17.12.2011 Android 4.0.3" sheetId="9" r:id="rId2"/>
-    <sheet name="22.8.2011" sheetId="7" r:id="rId3"/>
-    <sheet name="22.8.2011 VS" sheetId="8" r:id="rId4"/>
-    <sheet name="fast cursor" sheetId="6" r:id="rId5"/>
-    <sheet name="Preview3" sheetId="5" r:id="rId6"/>
-    <sheet name="VS" sheetId="2" r:id="rId7"/>
-    <sheet name="greenDAO" sheetId="4" r:id="rId8"/>
-    <sheet name="ORMLite" sheetId="1" r:id="rId9"/>
+    <sheet name="12.2.2012 VS Android 4.0.3" sheetId="11" r:id="rId1"/>
+    <sheet name="2.3 vs 4.0" sheetId="10" r:id="rId2"/>
+    <sheet name="17.12.2011 Android 4.0.3" sheetId="9" r:id="rId3"/>
+    <sheet name="22.8.2011" sheetId="7" r:id="rId4"/>
+    <sheet name="22.8.2011 VS" sheetId="8" r:id="rId5"/>
+    <sheet name="fast cursor" sheetId="6" r:id="rId6"/>
+    <sheet name="Preview3" sheetId="5" r:id="rId7"/>
+    <sheet name="VS" sheetId="2" r:id="rId8"/>
+    <sheet name="greenDAO" sheetId="4" r:id="rId9"/>
+    <sheet name="ORMLite" sheetId="1" r:id="rId10"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="66">
   <si>
     <t>100x Insert (one-by-one)</t>
   </si>
@@ -212,6 +213,15 @@
   <si>
     <t>2.3 vs. 4.0, Identity Scope</t>
   </si>
+  <si>
+    <t>ORMLite 4.24, Nexus S, Android 2.3</t>
+  </si>
+  <si>
+    <t>ORMLite 4.24, Nexus S, Android 4.0, 12.2.2012</t>
+  </si>
+  <si>
+    <t>ORMLite 4.34-SNAPSHOT, Nexus S, Android 4.0, 12.2.2012</t>
+  </si>
 </sst>
 </file>
 
@@ -273,7 +283,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -310,6 +320,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -324,7 +340,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -368,6 +384,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -386,7 +403,10 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Prozent" xfId="1" builtinId="5"/>
@@ -416,6 +436,250 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:view3D>
+      <c:rotX val="15"/>
+      <c:rotY val="20"/>
+      <c:rAngAx val="1"/>
+    </c:view3D>
+    <c:floor>
+      <c:thickness val="0"/>
+    </c:floor>
+    <c:sideWall>
+      <c:thickness val="0"/>
+    </c:sideWall>
+    <c:backWall>
+      <c:thickness val="0"/>
+    </c:backWall>
+    <c:plotArea>
+      <c:layout/>
+      <c:bar3DChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'12.2.2012 VS Android 4.0.3'!$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>greenDAO</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill>
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:srgbClr val="92D050"/>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:srgbClr val="9CB86E"/>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:srgbClr val="156B13"/>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'12.2.2012 VS Android 4.0.3'!$B$7:$D$7</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Load/s</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Update/s</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Insert/s</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'12.2.2012 VS Android 4.0.3'!$B$8:$D$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>17921.146953405019</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2272.7272727272725</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2847.380410022779</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'12.2.2012 VS Android 4.0.3'!$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ORMLite</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'12.2.2012 VS Android 4.0.3'!$B$7:$D$7</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Load/s</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Update/s</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Insert/s</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'12.2.2012 VS Android 4.0.3'!$B$9:$D$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>3958.8281868566905</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1413.2278123233464</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1641.4970453053184</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:shape val="box"/>
+        <c:axId val="169714176"/>
+        <c:axId val="173662208"/>
+        <c:axId val="0"/>
+      </c:bar3DChart>
+      <c:catAx>
+        <c:axId val="169714176"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="173662208"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="173662208"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="bg1">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="169714176"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="tr"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.72494510992182071"/>
+          <c:y val="0.11483085022535448"/>
+          <c:w val="0.14524883049299578"/>
+          <c:h val="0.12590366152011678"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="1"/>
+      <c:spPr>
+        <a:solidFill>
+          <a:schemeClr val="bg1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </c:spPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="de-DE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
     <c:title>
       <c:tx>
         <c:rich>
@@ -432,7 +696,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -517,11 +780,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="47193088"/>
-        <c:axId val="165012032"/>
+        <c:axId val="75278336"/>
+        <c:axId val="74550080"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="47193088"/>
+        <c:axId val="75278336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -530,7 +793,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="165012032"/>
+        <c:crossAx val="74550080"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -538,7 +801,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="165012032"/>
+        <c:axId val="74550080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -549,7 +812,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="47193088"/>
+        <c:crossAx val="75278336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.25"/>
@@ -572,317 +835,6 @@
       <a:endParaRPr lang="de-DE"/>
     </a:p>
   </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="de-DE"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:autoTitleDeleted val="0"/>
-    <c:view3D>
-      <c:rotX val="15"/>
-      <c:rotY val="20"/>
-      <c:rAngAx val="1"/>
-    </c:view3D>
-    <c:floor>
-      <c:thickness val="0"/>
-    </c:floor>
-    <c:sideWall>
-      <c:thickness val="0"/>
-    </c:sideWall>
-    <c:backWall>
-      <c:thickness val="0"/>
-    </c:backWall>
-    <c:plotArea>
-      <c:layout>
-        <c:manualLayout>
-          <c:layoutTarget val="inner"/>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.11423840769903762"/>
-          <c:y val="5.1400554097404488E-2"/>
-          <c:w val="0.84955314960629913"/>
-          <c:h val="0.77175014581510648"/>
-        </c:manualLayout>
-      </c:layout>
-      <c:bar3DChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'17.12.2011 Android 4.0.3'!$A$23</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Without Identity Scope</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:gradFill flip="none" rotWithShape="1">
-              <a:gsLst>
-                <a:gs pos="0">
-                  <a:srgbClr val="92D050">
-                    <a:shade val="30000"/>
-                    <a:satMod val="115000"/>
-                  </a:srgbClr>
-                </a:gs>
-                <a:gs pos="50000">
-                  <a:srgbClr val="92D050">
-                    <a:shade val="67500"/>
-                    <a:satMod val="115000"/>
-                  </a:srgbClr>
-                </a:gs>
-                <a:gs pos="100000">
-                  <a:srgbClr val="92D050">
-                    <a:shade val="100000"/>
-                    <a:satMod val="115000"/>
-                  </a:srgbClr>
-                </a:gs>
-              </a:gsLst>
-              <a:lin ang="2700000" scaled="1"/>
-              <a:tileRect/>
-            </a:gradFill>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>'17.12.2011 Android 4.0.3'!$G$22:$K$22</c:f>
-              <c:strCache>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>Loads/s</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Loads/s (2nd time)</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Inserts/s</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Updates/s</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Delete (all)/s</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'17.12.2011 Android 4.0.3'!$G$23:$K$23</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>17921.146953405016</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>17482.517482517484</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2847.380410022779</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2272.727272727273</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>13698.630136986301</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'17.12.2011 Android 4.0.3'!$A$24</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>With Identity Scope</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:gradFill flip="none" rotWithShape="1">
-              <a:gsLst>
-                <a:gs pos="0">
-                  <a:schemeClr val="accent3">
-                    <a:lumMod val="75000"/>
-                    <a:shade val="30000"/>
-                    <a:satMod val="115000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="50000">
-                  <a:schemeClr val="accent3">
-                    <a:lumMod val="75000"/>
-                    <a:shade val="67500"/>
-                    <a:satMod val="115000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="100000">
-                  <a:schemeClr val="accent3">
-                    <a:lumMod val="75000"/>
-                    <a:shade val="100000"/>
-                    <a:satMod val="115000"/>
-                  </a:schemeClr>
-                </a:gs>
-              </a:gsLst>
-              <a:lin ang="2700000" scaled="1"/>
-              <a:tileRect/>
-            </a:gradFill>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>'17.12.2011 Android 4.0.3'!$G$22:$K$22</c:f>
-              <c:strCache>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>Loads/s</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Loads/s (2nd time)</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Inserts/s</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Updates/s</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Delete (all)/s</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'17.12.2011 Android 4.0.3'!$G$24:$K$24</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>15243.902439024392</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>36764.705882352944</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2653.9278131634819</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2383.2221163012391</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>18939.39393939394</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="150"/>
-        <c:shape val="box"/>
-        <c:axId val="169918464"/>
-        <c:axId val="174206912"/>
-        <c:axId val="0"/>
-      </c:bar3DChart>
-      <c:catAx>
-        <c:axId val="169918464"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="174206912"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="174206912"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-          <c:max val="21000"/>
-          <c:min val="0"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="169918464"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-        <c:majorUnit val="4000"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout>
-        <c:manualLayout>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.72678109480919206"/>
-          <c:y val="9.8900522773982119E-2"/>
-          <c:w val="0.21301686210087048"/>
-          <c:h val="0.12100651445459654"/>
-        </c:manualLayout>
-      </c:layout>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:solidFill>
-          <a:schemeClr val="bg1">
-            <a:lumMod val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </c:spPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -941,7 +893,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'22.8.2011'!$A$23</c:f>
+              <c:f>'17.12.2011 Android 4.0.3'!$A$23</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -979,7 +931,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'22.8.2011'!$G$22:$K$22</c:f>
+              <c:f>'17.12.2011 Android 4.0.3'!$G$22:$K$22</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -1002,24 +954,24 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'22.8.2011'!$G$23:$K$23</c:f>
+              <c:f>'17.12.2011 Android 4.0.3'!$G$23:$K$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>12658.227848101265</c:v>
+                  <c:v>17921.146953405016</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>14925.373134328358</c:v>
+                  <c:v>17482.517482517484</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5707.7625570776254</c:v>
+                  <c:v>2847.380410022779</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5015.0451354062188</c:v>
+                  <c:v>2272.727272727273</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>11111.111111111111</c:v>
+                  <c:v>13698.630136986301</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1030,7 +982,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'22.8.2011'!$A$24</c:f>
+              <c:f>'17.12.2011 Android 4.0.3'!$A$24</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1071,7 +1023,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'22.8.2011'!$G$22:$K$22</c:f>
+              <c:f>'17.12.2011 Android 4.0.3'!$G$22:$K$22</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -1094,24 +1046,24 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'22.8.2011'!$G$24:$K$24</c:f>
+              <c:f>'17.12.2011 Android 4.0.3'!$G$24:$K$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>11655.011655011656</c:v>
+                  <c:v>15243.902439024392</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>29761.90476190476</c:v>
+                  <c:v>36764.705882352944</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5574.1360089186173</c:v>
+                  <c:v>2653.9278131634819</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4625.3469010175768</c:v>
+                  <c:v>2383.2221163012391</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>10482.180293501047</c:v>
+                  <c:v>18939.39393939394</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1127,12 +1079,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="165206528"/>
-        <c:axId val="165229056"/>
+        <c:axId val="76255232"/>
+        <c:axId val="74551808"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="165206528"/>
+        <c:axId val="76255232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1142,7 +1094,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="165229056"/>
+        <c:crossAx val="74551808"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1150,7 +1102,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="165229056"/>
+        <c:axId val="74551808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="21000"/>
@@ -1163,7 +1115,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="165206528"/>
+        <c:crossAx val="76255232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="4000"/>
@@ -1232,7 +1184,17 @@
       <c:thickness val="0"/>
     </c:backWall>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.11423840769903762"/>
+          <c:y val="5.1400554097404488E-2"/>
+          <c:w val="0.84955314960629913"/>
+          <c:h val="0.77175014581510648"/>
+        </c:manualLayout>
+      </c:layout>
       <c:bar3DChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
@@ -1242,63 +1204,85 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'22.8.2011 VS'!$A$8</c:f>
+              <c:f>'22.8.2011'!$A$23</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>greenDAO</c:v>
+                  <c:v>Without Identity Scope</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:gradFill>
+            <a:gradFill flip="none" rotWithShape="1">
               <a:gsLst>
                 <a:gs pos="0">
-                  <a:srgbClr val="92D050"/>
+                  <a:srgbClr val="92D050">
+                    <a:shade val="30000"/>
+                    <a:satMod val="115000"/>
+                  </a:srgbClr>
                 </a:gs>
                 <a:gs pos="50000">
-                  <a:srgbClr val="9CB86E"/>
+                  <a:srgbClr val="92D050">
+                    <a:shade val="67500"/>
+                    <a:satMod val="115000"/>
+                  </a:srgbClr>
                 </a:gs>
                 <a:gs pos="100000">
-                  <a:srgbClr val="156B13"/>
+                  <a:srgbClr val="92D050">
+                    <a:shade val="100000"/>
+                    <a:satMod val="115000"/>
+                  </a:srgbClr>
                 </a:gs>
               </a:gsLst>
-              <a:lin ang="5400000" scaled="0"/>
+              <a:lin ang="2700000" scaled="1"/>
+              <a:tileRect/>
             </a:gradFill>
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'22.8.2011 VS'!$B$7:$D$7</c:f>
+              <c:f>'22.8.2011'!$G$22:$K$22</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>Insert/s</c:v>
+                  <c:v>Loads/s</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Update/s</c:v>
+                  <c:v>Loads/s (2nd time)</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Load/s</c:v>
+                  <c:v>Inserts/s</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Updates/s</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Delete (all)/s</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'22.8.2011 VS'!$B$8:$D$8</c:f>
+              <c:f>'22.8.2011'!$G$23:$K$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>5707.7625570776263</c:v>
+                  <c:v>12658.227848101265</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>14925.373134328358</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5707.7625570776254</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>5015.0451354062188</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>12658.227848101265</c:v>
+                <c:pt idx="4">
+                  <c:v>11111.111111111111</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1309,47 +1293,88 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'22.8.2011 VS'!$A$9</c:f>
+              <c:f>'22.8.2011'!$A$24</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>ORMLite</c:v>
+                  <c:v>With Identity Scope</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:gradFill flip="none" rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent3">
+                    <a:lumMod val="75000"/>
+                    <a:shade val="30000"/>
+                    <a:satMod val="115000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent3">
+                    <a:lumMod val="75000"/>
+                    <a:shade val="67500"/>
+                    <a:satMod val="115000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent3">
+                    <a:lumMod val="75000"/>
+                    <a:shade val="100000"/>
+                    <a:satMod val="115000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="2700000" scaled="1"/>
+              <a:tileRect/>
+            </a:gradFill>
+          </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'22.8.2011 VS'!$B$7:$D$7</c:f>
+              <c:f>'22.8.2011'!$G$22:$K$22</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>Insert/s</c:v>
+                  <c:v>Loads/s</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Update/s</c:v>
+                  <c:v>Loads/s (2nd time)</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Load/s</c:v>
+                  <c:v>Inserts/s</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Updates/s</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Delete (all)/s</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'22.8.2011 VS'!$B$9:$D$9</c:f>
+              <c:f>'22.8.2011'!$G$24:$K$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>2223.2103156958647</c:v>
+                  <c:v>11655.011655011656</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2190.1007446342533</c:v>
+                  <c:v>29761.90476190476</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2790.1785714285716</c:v>
+                  <c:v>5574.1360089186173</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4625.3469010175768</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10482.180293501047</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1365,21 +1390,22 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="166469120"/>
-        <c:axId val="165231360"/>
+        <c:axId val="76257280"/>
+        <c:axId val="74554112"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="166469120"/>
+        <c:axId val="76257280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="165231360"/>
+        <c:crossAx val="74554112"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1387,45 +1413,38 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="165231360"/>
+        <c:axId val="74554112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="21000"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln>
-              <a:solidFill>
-                <a:schemeClr val="bg1">
-                  <a:lumMod val="75000"/>
-                </a:schemeClr>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
+        <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="166469120"/>
+        <c:crossAx val="76257280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
+        <c:majorUnit val="4000"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="tr"/>
+      <c:legendPos val="r"/>
       <c:layout>
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.2640702099737533"/>
-          <c:y val="0.12260536398467432"/>
-          <c:w val="0.14524883049299578"/>
-          <c:h val="0.12590366152011678"/>
+          <c:x val="0.72678109480919206"/>
+          <c:y val="9.8900522773982119E-2"/>
+          <c:w val="0.21301686210087048"/>
+          <c:h val="0.12100651445459654"/>
         </c:manualLayout>
       </c:layout>
-      <c:overlay val="1"/>
+      <c:overlay val="0"/>
       <c:spPr>
         <a:solidFill>
           <a:schemeClr val="bg1">
@@ -1476,17 +1495,7 @@
       <c:thickness val="0"/>
     </c:backWall>
     <c:plotArea>
-      <c:layout>
-        <c:manualLayout>
-          <c:layoutTarget val="inner"/>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.11423840769903762"/>
-          <c:y val="5.1400554097404488E-2"/>
-          <c:w val="0.84955314960629913"/>
-          <c:h val="0.77175014581510648"/>
-        </c:manualLayout>
-      </c:layout>
+      <c:layout/>
       <c:bar3DChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
@@ -1496,85 +1505,63 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'fast cursor'!$A$23</c:f>
+              <c:f>'22.8.2011 VS'!$A$8</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Without Identity Scope</c:v>
+                  <c:v>greenDAO</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:gradFill flip="none" rotWithShape="1">
+            <a:gradFill>
               <a:gsLst>
                 <a:gs pos="0">
-                  <a:srgbClr val="92D050">
-                    <a:shade val="30000"/>
-                    <a:satMod val="115000"/>
-                  </a:srgbClr>
+                  <a:srgbClr val="92D050"/>
                 </a:gs>
                 <a:gs pos="50000">
-                  <a:srgbClr val="92D050">
-                    <a:shade val="67500"/>
-                    <a:satMod val="115000"/>
-                  </a:srgbClr>
+                  <a:srgbClr val="9CB86E"/>
                 </a:gs>
                 <a:gs pos="100000">
-                  <a:srgbClr val="92D050">
-                    <a:shade val="100000"/>
-                    <a:satMod val="115000"/>
-                  </a:srgbClr>
+                  <a:srgbClr val="156B13"/>
                 </a:gs>
               </a:gsLst>
-              <a:lin ang="2700000" scaled="1"/>
-              <a:tileRect/>
+              <a:lin ang="5400000" scaled="0"/>
             </a:gradFill>
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'fast cursor'!$G$22:$K$22</c:f>
+              <c:f>'22.8.2011 VS'!$B$7:$D$7</c:f>
               <c:strCache>
-                <c:ptCount val="5"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>Loads/s</c:v>
+                  <c:v>Insert/s</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Loads/s (2nd time)</c:v>
+                  <c:v>Update/s</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Loads/s (long key)</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Loads/s (2nd, long key)</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Loads/s (Object key)</c:v>
+                  <c:v>Load/s</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'fast cursor'!$G$23:$K$23</c:f>
+              <c:f>'22.8.2011 VS'!$B$8:$D$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>10683.760683760685</c:v>
+                  <c:v>5707.7625570776263</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>15527.950310559005</c:v>
+                  <c:v>5015.0451354062188</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>12658.227848101265</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1585,88 +1572,47 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'fast cursor'!$A$24</c:f>
+              <c:f>'22.8.2011 VS'!$A$9</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>With Identity Scope</c:v>
+                  <c:v>ORMLite</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:spPr>
-            <a:gradFill flip="none" rotWithShape="1">
-              <a:gsLst>
-                <a:gs pos="0">
-                  <a:schemeClr val="accent3">
-                    <a:lumMod val="75000"/>
-                    <a:shade val="30000"/>
-                    <a:satMod val="115000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="50000">
-                  <a:schemeClr val="accent3">
-                    <a:lumMod val="75000"/>
-                    <a:shade val="67500"/>
-                    <a:satMod val="115000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="100000">
-                  <a:schemeClr val="accent3">
-                    <a:lumMod val="75000"/>
-                    <a:shade val="100000"/>
-                    <a:satMod val="115000"/>
-                  </a:schemeClr>
-                </a:gs>
-              </a:gsLst>
-              <a:lin ang="2700000" scaled="1"/>
-              <a:tileRect/>
-            </a:gradFill>
-          </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'fast cursor'!$G$22:$K$22</c:f>
+              <c:f>'22.8.2011 VS'!$B$7:$D$7</c:f>
               <c:strCache>
-                <c:ptCount val="5"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>Loads/s</c:v>
+                  <c:v>Insert/s</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Loads/s (2nd time)</c:v>
+                  <c:v>Update/s</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Loads/s (long key)</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Loads/s (2nd, long key)</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Loads/s (Object key)</c:v>
+                  <c:v>Load/s</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'fast cursor'!$G$24:$K$24</c:f>
+              <c:f>'22.8.2011 VS'!$B$9:$D$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>7418.3976261127591</c:v>
+                  <c:v>2223.2103156958647</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>24509.803921568629</c:v>
+                  <c:v>2190.1007446342533</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9803.9215686274511</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>25510.204081632652</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>9746.5886939571155</c:v>
+                  <c:v>2790.1785714285716</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1682,22 +1628,21 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="169772544"/>
-        <c:axId val="167912576"/>
+        <c:axId val="89329664"/>
+        <c:axId val="89539712"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="169772544"/>
+        <c:axId val="89329664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="167912576"/>
+        <c:crossAx val="89539712"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1705,38 +1650,45 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="167912576"/>
+        <c:axId val="89539712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="21000"/>
-          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
-        <c:majorGridlines/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="bg1">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="169772544"/>
+        <c:crossAx val="89329664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
-        <c:majorUnit val="4000"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="r"/>
+      <c:legendPos val="tr"/>
       <c:layout>
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.77282426027681794"/>
-          <c:y val="4.2020563725444993E-2"/>
-          <c:w val="0.21301686210087048"/>
-          <c:h val="0.12100651445459654"/>
+          <c:x val="0.2640702099737533"/>
+          <c:y val="0.12260536398467432"/>
+          <c:w val="0.14524883049299578"/>
+          <c:h val="0.12590366152011678"/>
         </c:manualLayout>
       </c:layout>
-      <c:overlay val="0"/>
+      <c:overlay val="1"/>
       <c:spPr>
         <a:solidFill>
           <a:schemeClr val="bg1">
@@ -1807,7 +1759,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Preview3!$A$23</c:f>
+              <c:f>'fast cursor'!$A$23</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1845,7 +1797,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Preview3!$G$22:$K$22</c:f>
+              <c:f>'fast cursor'!$G$22:$K$22</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -1855,37 +1807,37 @@
                   <c:v>Loads/s (2nd time)</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Inserts/s</c:v>
+                  <c:v>Loads/s (long key)</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Updates/s</c:v>
+                  <c:v>Loads/s (2nd, long key)</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Delete (all)/s</c:v>
+                  <c:v>Loads/s (Object key)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Preview3!$G$23:$K$23</c:f>
+              <c:f>'fast cursor'!$G$23:$K$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>8103.7277147487839</c:v>
+                  <c:v>10683.760683760685</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>11520.737327188941</c:v>
+                  <c:v>15527.950310559005</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5567.9287305122498</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5422.9934924078088</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>15384.615384615385</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1896,7 +1848,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Preview3!$A$24</c:f>
+              <c:f>'fast cursor'!$A$24</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1937,7 +1889,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Preview3!$G$22:$K$22</c:f>
+              <c:f>'fast cursor'!$G$22:$K$22</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -1947,37 +1899,37 @@
                   <c:v>Loads/s (2nd time)</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Inserts/s</c:v>
+                  <c:v>Loads/s (long key)</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Updates/s</c:v>
+                  <c:v>Loads/s (2nd, long key)</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Delete (all)/s</c:v>
+                  <c:v>Loads/s (Object key)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Preview3!$G$24:$K$24</c:f>
+              <c:f>'fast cursor'!$G$24:$K$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>5144.032921810699</c:v>
+                  <c:v>7418.3976261127591</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>21008.403361344539</c:v>
+                  <c:v>24509.803921568629</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4314.0638481449523</c:v>
+                  <c:v>9803.9215686274511</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4990.0199600798396</c:v>
+                  <c:v>25510.204081632652</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>13774.104683195594</c:v>
+                  <c:v>9746.5886939571155</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1993,12 +1945,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="166468608"/>
-        <c:axId val="167914880"/>
+        <c:axId val="89331712"/>
+        <c:axId val="89542016"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="166468608"/>
+        <c:axId val="89331712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2008,7 +1960,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="167914880"/>
+        <c:crossAx val="89542016"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2016,7 +1968,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="167914880"/>
+        <c:axId val="89542016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="21000"/>
@@ -2029,7 +1981,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="166468608"/>
+        <c:crossAx val="89331712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="4000"/>
@@ -2041,8 +1993,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.72678109480919206"/>
-          <c:y val="9.8900522773982119E-2"/>
+          <c:x val="0.77282426027681794"/>
+          <c:y val="4.2020563725444993E-2"/>
           <c:w val="0.21301686210087048"/>
           <c:h val="0.12100651445459654"/>
         </c:manualLayout>
@@ -2098,6 +2050,317 @@
       <c:thickness val="0"/>
     </c:backWall>
     <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.11423840769903762"/>
+          <c:y val="5.1400554097404488E-2"/>
+          <c:w val="0.84955314960629913"/>
+          <c:h val="0.77175014581510648"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:bar3DChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Preview3!$A$23</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Without Identity Scope</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill flip="none" rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:srgbClr val="92D050">
+                    <a:shade val="30000"/>
+                    <a:satMod val="115000"/>
+                  </a:srgbClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:srgbClr val="92D050">
+                    <a:shade val="67500"/>
+                    <a:satMod val="115000"/>
+                  </a:srgbClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:srgbClr val="92D050">
+                    <a:shade val="100000"/>
+                    <a:satMod val="115000"/>
+                  </a:srgbClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="2700000" scaled="1"/>
+              <a:tileRect/>
+            </a:gradFill>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Preview3!$G$22:$K$22</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Loads/s</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Loads/s (2nd time)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Inserts/s</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Updates/s</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Delete (all)/s</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Preview3!$G$23:$K$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>8103.7277147487839</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11520.737327188941</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5567.9287305122498</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5422.9934924078088</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>15384.615384615385</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Preview3!$A$24</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>With Identity Scope</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill flip="none" rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent3">
+                    <a:lumMod val="75000"/>
+                    <a:shade val="30000"/>
+                    <a:satMod val="115000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent3">
+                    <a:lumMod val="75000"/>
+                    <a:shade val="67500"/>
+                    <a:satMod val="115000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent3">
+                    <a:lumMod val="75000"/>
+                    <a:shade val="100000"/>
+                    <a:satMod val="115000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="2700000" scaled="1"/>
+              <a:tileRect/>
+            </a:gradFill>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Preview3!$G$22:$K$22</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Loads/s</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Loads/s (2nd time)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Inserts/s</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Updates/s</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Delete (all)/s</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Preview3!$G$24:$K$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>5144.032921810699</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>21008.403361344539</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4314.0638481449523</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4990.0199600798396</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>13774.104683195594</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:shape val="box"/>
+        <c:axId val="89448448"/>
+        <c:axId val="89544320"/>
+        <c:axId val="0"/>
+      </c:bar3DChart>
+      <c:catAx>
+        <c:axId val="89448448"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="89544320"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="89544320"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="21000"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="89448448"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:majorUnit val="4000"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.72678109480919206"/>
+          <c:y val="9.8900522773982119E-2"/>
+          <c:w val="0.21301686210087048"/>
+          <c:h val="0.12100651445459654"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:solidFill>
+          <a:schemeClr val="bg1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </c:spPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="de-DE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:view3D>
+      <c:rotX val="15"/>
+      <c:rotY val="20"/>
+      <c:rAngAx val="1"/>
+    </c:view3D>
+    <c:floor>
+      <c:thickness val="0"/>
+    </c:floor>
+    <c:sideWall>
+      <c:thickness val="0"/>
+    </c:sideWall>
+    <c:backWall>
+      <c:thickness val="0"/>
+    </c:backWall>
+    <c:plotArea>
       <c:layout/>
       <c:bar3DChart>
         <c:barDir val="col"/>
@@ -2231,12 +2494,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="165207040"/>
-        <c:axId val="167917184"/>
+        <c:axId val="75279360"/>
+        <c:axId val="89677824"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="165207040"/>
+        <c:axId val="75279360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2245,7 +2508,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="167917184"/>
+        <c:crossAx val="89677824"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2253,7 +2516,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="167917184"/>
+        <c:axId val="89677824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2274,7 +2537,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="165207040"/>
+        <c:crossAx val="75279360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2316,21 +2579,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>314324</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>119062</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>647699</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>523875</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>466725</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Diagramm 2"/>
-        <xdr:cNvGraphicFramePr/>
+        <xdr:cNvPr id="2" name="Diagramm 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -2351,23 +2616,21 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>723899</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>166686</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>314324</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>119062</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>476249</xdr:colOff>
-      <xdr:row>59</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Diagramm 1"/>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks/>
-        </xdr:cNvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Diagramm 2"/>
+        <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -2425,16 +2688,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>647699</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>723899</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>166686</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>466725</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>476249</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2462,16 +2725,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>704849</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>4761</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>647699</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>457199</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>180974</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>466725</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2513,6 +2776,43 @@
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Diagramm 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>704849</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>4761</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>457199</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>180974</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Diagramm 1"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2530,7 +2830,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -2852,6 +3152,629 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.42578125" style="1"/>
+    <col min="2" max="2" width="12.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="14" style="1" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="8.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="13" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="11.42578125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="B1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1">
+        <f>'17.12.2011 Android 4.0.3'!D8</f>
+        <v>8567.6</v>
+      </c>
+      <c r="C2" s="1">
+        <f>'17.12.2011 Android 4.0.3'!E8</f>
+        <v>8302.4</v>
+      </c>
+      <c r="D2" s="1">
+        <f>'17.12.2011 Android 4.0.3'!I8</f>
+        <v>351.2</v>
+      </c>
+      <c r="E2" s="1">
+        <f>'17.12.2011 Android 4.0.3'!J8</f>
+        <v>440</v>
+      </c>
+      <c r="F2" s="1">
+        <f>'17.12.2011 Android 4.0.3'!G8</f>
+        <v>55.8</v>
+      </c>
+      <c r="G2" s="5">
+        <f>greenDAO!F7</f>
+        <v>153.80000000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="1">
+        <f>ORMLite!B26</f>
+        <v>7757.6</v>
+      </c>
+      <c r="C3" s="1">
+        <f>ORMLite!C26</f>
+        <v>7565.4</v>
+      </c>
+      <c r="D3" s="1">
+        <f>ORMLite!D26</f>
+        <v>609.20000000000005</v>
+      </c>
+      <c r="E3" s="1">
+        <f>ORMLite!E26</f>
+        <v>707.6</v>
+      </c>
+      <c r="F3" s="1">
+        <f>ORMLite!F26</f>
+        <v>252.6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="1">
+        <f>1000*1000/F2</f>
+        <v>17921.146953405019</v>
+      </c>
+      <c r="C8" s="1">
+        <f t="shared" ref="B8:E9" si="0">1000*1000/E2</f>
+        <v>2272.7272727272725</v>
+      </c>
+      <c r="D8" s="1">
+        <f>1000*1000/D2</f>
+        <v>2847.380410022779</v>
+      </c>
+      <c r="E8" s="1">
+        <f t="shared" si="0"/>
+        <v>6501.9505851755521</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="1">
+        <f>1000*1000/F3</f>
+        <v>3958.8281868566905</v>
+      </c>
+      <c r="C9" s="1">
+        <f t="shared" si="0"/>
+        <v>1413.2278123233464</v>
+      </c>
+      <c r="D9" s="1">
+        <f>1000*1000/D3</f>
+        <v>1641.4970453053184</v>
+      </c>
+      <c r="E9" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E10" s="5"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E11" s="5"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E12" s="5"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E13" s="5"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B14" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E14" s="4"/>
+    </row>
+    <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" s="1">
+        <f>D3/D2</f>
+        <v>1.7346241457858771</v>
+      </c>
+      <c r="C15" s="1">
+        <f>E3/E2</f>
+        <v>1.6081818181818182</v>
+      </c>
+      <c r="D15" s="1">
+        <f>F3/F2</f>
+        <v>4.5268817204301079</v>
+      </c>
+      <c r="E15" s="5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F26"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.42578125" style="1"/>
+    <col min="2" max="2" width="13.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="11.42578125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+    </row>
+    <row r="2" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B3" s="1">
+        <v>8540</v>
+      </c>
+      <c r="C3" s="1">
+        <v>8895</v>
+      </c>
+      <c r="D3" s="1">
+        <v>426</v>
+      </c>
+      <c r="E3" s="1">
+        <v>414</v>
+      </c>
+      <c r="F3" s="1">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B4" s="1">
+        <v>8575</v>
+      </c>
+      <c r="C4" s="1">
+        <v>8117</v>
+      </c>
+      <c r="D4" s="1">
+        <v>506</v>
+      </c>
+      <c r="E4" s="1">
+        <v>489</v>
+      </c>
+      <c r="F4" s="1">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B5" s="1">
+        <v>7593</v>
+      </c>
+      <c r="C5" s="1">
+        <v>8881</v>
+      </c>
+      <c r="D5" s="1">
+        <v>428</v>
+      </c>
+      <c r="E5" s="1">
+        <v>446</v>
+      </c>
+      <c r="F5" s="1">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B6" s="1">
+        <v>9451</v>
+      </c>
+      <c r="C6" s="1">
+        <v>7448</v>
+      </c>
+      <c r="D6" s="1">
+        <v>436</v>
+      </c>
+      <c r="E6" s="1">
+        <v>498</v>
+      </c>
+      <c r="F6" s="1">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B7" s="1">
+        <v>7955</v>
+      </c>
+      <c r="C7" s="1">
+        <v>8812</v>
+      </c>
+      <c r="D7" s="1">
+        <v>453</v>
+      </c>
+      <c r="E7" s="1">
+        <v>436</v>
+      </c>
+      <c r="F7" s="1">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="2">
+        <f>AVERAGE(B3:B7)</f>
+        <v>8422.7999999999993</v>
+      </c>
+      <c r="C8" s="2">
+        <f>AVERAGE(C3:C7)</f>
+        <v>8430.6</v>
+      </c>
+      <c r="D8" s="2">
+        <f>AVERAGE(D3:D7)</f>
+        <v>449.8</v>
+      </c>
+      <c r="E8" s="2">
+        <f>AVERAGE(E3:E7)</f>
+        <v>456.6</v>
+      </c>
+      <c r="F8" s="2">
+        <f>AVERAGE(F3:F7)</f>
+        <v>358.4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="B10" s="22"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="22"/>
+      <c r="E10" s="22"/>
+      <c r="F10" s="22"/>
+    </row>
+    <row r="11" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="B11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B12" s="1">
+        <v>7796</v>
+      </c>
+      <c r="C12" s="1">
+        <v>9179</v>
+      </c>
+      <c r="D12" s="1">
+        <v>628</v>
+      </c>
+      <c r="E12" s="1">
+        <v>612</v>
+      </c>
+      <c r="F12" s="1">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B13" s="1">
+        <v>8550</v>
+      </c>
+      <c r="C13" s="1">
+        <v>8745</v>
+      </c>
+      <c r="D13" s="1">
+        <v>528</v>
+      </c>
+      <c r="E13" s="1">
+        <v>555</v>
+      </c>
+      <c r="F13" s="1">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B14" s="1">
+        <v>6867</v>
+      </c>
+      <c r="C14" s="1">
+        <v>7142</v>
+      </c>
+      <c r="D14" s="1">
+        <v>526</v>
+      </c>
+      <c r="E14" s="1">
+        <v>520</v>
+      </c>
+      <c r="F14" s="1">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B15" s="1">
+        <v>8412</v>
+      </c>
+      <c r="C15" s="1">
+        <v>7370</v>
+      </c>
+      <c r="D15" s="1">
+        <v>514</v>
+      </c>
+      <c r="E15" s="1">
+        <v>529</v>
+      </c>
+      <c r="F15" s="1">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B16" s="1">
+        <v>9271</v>
+      </c>
+      <c r="C16" s="1">
+        <v>4730</v>
+      </c>
+      <c r="D16" s="1">
+        <v>497</v>
+      </c>
+      <c r="E16" s="1">
+        <v>536</v>
+      </c>
+      <c r="F16" s="1">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B17" s="2">
+        <f>AVERAGE(B12:B16)</f>
+        <v>8179.2</v>
+      </c>
+      <c r="C17" s="2">
+        <f>AVERAGE(C12:C16)</f>
+        <v>7433.2</v>
+      </c>
+      <c r="D17" s="2">
+        <f>AVERAGE(D12:D16)</f>
+        <v>538.6</v>
+      </c>
+      <c r="E17" s="2">
+        <f>AVERAGE(E12:E16)</f>
+        <v>550.4</v>
+      </c>
+      <c r="F17" s="2">
+        <f>AVERAGE(F12:F16)</f>
+        <v>272.2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="23" t="s">
+        <v>65</v>
+      </c>
+      <c r="B19" s="22"/>
+      <c r="C19" s="22"/>
+      <c r="D19" s="22"/>
+      <c r="E19" s="22"/>
+      <c r="F19" s="22"/>
+    </row>
+    <row r="20" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="B20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B21" s="1">
+        <v>7432</v>
+      </c>
+      <c r="C21" s="1">
+        <v>7280</v>
+      </c>
+      <c r="D21" s="1">
+        <v>656</v>
+      </c>
+      <c r="E21" s="1">
+        <v>575</v>
+      </c>
+      <c r="F21" s="1">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B22" s="1">
+        <v>8429</v>
+      </c>
+      <c r="C22" s="1">
+        <v>9270</v>
+      </c>
+      <c r="D22" s="1">
+        <v>526</v>
+      </c>
+      <c r="E22" s="1">
+        <v>561</v>
+      </c>
+      <c r="F22" s="1">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B23" s="1">
+        <v>6754</v>
+      </c>
+      <c r="C23" s="1">
+        <v>8512</v>
+      </c>
+      <c r="D23" s="1">
+        <v>606</v>
+      </c>
+      <c r="E23" s="1">
+        <v>566</v>
+      </c>
+      <c r="F23" s="1">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B24" s="1">
+        <v>8676</v>
+      </c>
+      <c r="C24" s="1">
+        <v>4683</v>
+      </c>
+      <c r="D24" s="1">
+        <v>558</v>
+      </c>
+      <c r="E24" s="1">
+        <v>553</v>
+      </c>
+      <c r="F24" s="1">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B25" s="1">
+        <v>7497</v>
+      </c>
+      <c r="C25" s="1">
+        <v>8082</v>
+      </c>
+      <c r="D25" s="1">
+        <v>700</v>
+      </c>
+      <c r="E25" s="1">
+        <v>1283</v>
+      </c>
+      <c r="F25" s="1">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B26" s="2">
+        <f>AVERAGE(B21:B25)</f>
+        <v>7757.6</v>
+      </c>
+      <c r="C26" s="2">
+        <f>AVERAGE(C21:C25)</f>
+        <v>7565.4</v>
+      </c>
+      <c r="D26" s="2">
+        <f>AVERAGE(D21:D25)</f>
+        <v>609.20000000000005</v>
+      </c>
+      <c r="E26" s="2">
+        <f>AVERAGE(E21:E25)</f>
+        <v>707.6</v>
+      </c>
+      <c r="F26" s="2">
+        <f>AVERAGE(F21:F25)</f>
+        <v>252.6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
@@ -2864,23 +3787,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="16" t="s">
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="16"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
     </row>
     <row r="2" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="15" t="s">
         <v>56</v>
       </c>
       <c r="B2" s="3" t="s">
@@ -3071,43 +3994,43 @@
         <v>61</v>
       </c>
       <c r="B8" s="9">
-        <f>B5/B3</f>
+        <f t="shared" ref="B8:K8" si="0">B5/B3</f>
         <v>0.68307180218735142</v>
       </c>
       <c r="C8" s="9">
-        <f>C5/C3</f>
+        <f t="shared" si="0"/>
         <v>0.67457464653726329</v>
       </c>
       <c r="D8" s="9">
-        <f>D5/D3</f>
+        <f t="shared" si="0"/>
         <v>0.9943274662682664</v>
       </c>
       <c r="E8" s="9">
-        <f>E5/E3</f>
+        <f t="shared" si="0"/>
         <v>0.98077664289843902</v>
       </c>
       <c r="F8" s="9">
-        <f>F5/F3</f>
+        <f t="shared" si="0"/>
         <v>1.0992828134450876</v>
       </c>
       <c r="G8" s="9">
-        <f>G5/G3</f>
+        <f t="shared" si="0"/>
         <v>1.4157706093189966</v>
       </c>
       <c r="H8" s="9">
-        <f>H5/H3</f>
+        <f t="shared" si="0"/>
         <v>1.1713286713286712</v>
       </c>
       <c r="I8" s="9">
-        <f>I5/I3</f>
+        <f t="shared" si="0"/>
         <v>0.49886104783599089</v>
       </c>
       <c r="J8" s="9">
-        <f>J5/J3</f>
+        <f t="shared" si="0"/>
         <v>0.45318181818181819</v>
       </c>
       <c r="K8" s="9">
-        <f>K5/K3</f>
+        <f t="shared" si="0"/>
         <v>1.2328767123287672</v>
       </c>
     </row>
@@ -3120,39 +4043,39 @@
         <v>0.67346938775510212</v>
       </c>
       <c r="C9" s="9">
-        <f t="shared" ref="C9:K9" si="0">C6/C4</f>
+        <f t="shared" ref="C9:K9" si="1">C6/C4</f>
         <v>0.79166666666666663</v>
       </c>
       <c r="D9" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.90201045528867185</v>
       </c>
       <c r="E9" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.1272204959840535</v>
       </c>
       <c r="F9" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.84125770320723314</v>
       </c>
       <c r="G9" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.3079268292682928</v>
       </c>
       <c r="H9" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.2352941176470589</v>
       </c>
       <c r="I9" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.47611464968152867</v>
       </c>
       <c r="J9" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.51525262154432783</v>
       </c>
       <c r="K9" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.8068181818181821</v>
       </c>
     </row>
@@ -3167,12 +4090,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3192,26 +4115,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="16" t="s">
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="16"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
     </row>
     <row r="2" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="19"/>
+      <c r="A2" s="20"/>
       <c r="B2" s="3" t="s">
         <v>22</v>
       </c>
@@ -3244,7 +4167,7 @@
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="19"/>
+      <c r="A3" s="20"/>
       <c r="B3" s="14">
         <v>969</v>
       </c>
@@ -3277,7 +4200,7 @@
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="19"/>
+      <c r="A4" s="20"/>
       <c r="B4" s="14">
         <v>813</v>
       </c>
@@ -3310,7 +4233,7 @@
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="19"/>
+      <c r="A5" s="20"/>
       <c r="B5" s="14">
         <v>816</v>
       </c>
@@ -3343,7 +4266,7 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="19"/>
+      <c r="A6" s="20"/>
       <c r="B6" s="14">
         <v>805</v>
       </c>
@@ -3376,7 +4299,7 @@
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="19"/>
+      <c r="A7" s="20"/>
       <c r="B7" s="14">
         <v>803</v>
       </c>
@@ -3409,7 +4332,7 @@
       </c>
     </row>
     <row r="8" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="19"/>
+      <c r="A8" s="20"/>
       <c r="B8" s="2">
         <f t="shared" ref="B8:K8" si="0">AVERAGE(B3:B7)</f>
         <v>841.2</v>
@@ -3456,26 +4379,26 @@
       <c r="C9" s="14"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="19" t="s">
+      <c r="A10" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="B10" s="20" t="s">
+      <c r="B10" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="20"/>
-      <c r="D10" s="20"/>
-      <c r="E10" s="20"/>
-      <c r="F10" s="20"/>
-      <c r="G10" s="16" t="s">
+      <c r="C10" s="21"/>
+      <c r="D10" s="21"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="21"/>
+      <c r="G10" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="H10" s="16"/>
-      <c r="I10" s="16"/>
-      <c r="J10" s="16"/>
-      <c r="K10" s="16"/>
+      <c r="H10" s="17"/>
+      <c r="I10" s="17"/>
+      <c r="J10" s="17"/>
+      <c r="K10" s="17"/>
     </row>
     <row r="11" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="19"/>
+      <c r="A11" s="20"/>
       <c r="B11" s="3" t="s">
         <v>22</v>
       </c>
@@ -3508,7 +4431,7 @@
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="19"/>
+      <c r="A12" s="20"/>
       <c r="B12" s="14">
         <v>1125</v>
       </c>
@@ -3541,7 +4464,7 @@
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="19"/>
+      <c r="A13" s="20"/>
       <c r="B13" s="14">
         <v>884</v>
       </c>
@@ -3574,7 +4497,7 @@
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="19"/>
+      <c r="A14" s="20"/>
       <c r="B14" s="14">
         <v>930</v>
       </c>
@@ -3607,7 +4530,7 @@
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="19"/>
+      <c r="A15" s="20"/>
       <c r="B15" s="14">
         <v>884</v>
       </c>
@@ -3640,7 +4563,7 @@
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="19"/>
+      <c r="A16" s="20"/>
       <c r="B16" s="14">
         <v>881</v>
       </c>
@@ -3673,7 +4596,7 @@
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="19"/>
+      <c r="A17" s="20"/>
       <c r="B17" s="2">
         <f t="shared" ref="B17:K17" si="1">AVERAGE(B12:B16)</f>
         <v>940.8</v>
@@ -3756,20 +4679,20 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="7"/>
-      <c r="B21" s="15" t="s">
+      <c r="B21" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="15"/>
-      <c r="D21" s="15"/>
-      <c r="E21" s="15"/>
-      <c r="F21" s="15"/>
-      <c r="G21" s="16" t="s">
+      <c r="C21" s="16"/>
+      <c r="D21" s="16"/>
+      <c r="E21" s="16"/>
+      <c r="F21" s="16"/>
+      <c r="G21" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="H21" s="16"/>
-      <c r="I21" s="16"/>
-      <c r="J21" s="16"/>
-      <c r="K21" s="16"/>
+      <c r="H21" s="17"/>
+      <c r="I21" s="17"/>
+      <c r="J21" s="17"/>
+      <c r="K21" s="17"/>
     </row>
     <row r="22" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="7"/>
@@ -3940,18 +4863,18 @@
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B27" s="17" t="s">
+      <c r="B27" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="C27" s="17"/>
-      <c r="D27" s="17"/>
-      <c r="E27" s="17"/>
-      <c r="F27" s="17"/>
-      <c r="G27" s="17"/>
-      <c r="H27" s="17"/>
-      <c r="I27" s="17"/>
-      <c r="J27" s="17"/>
-      <c r="K27" s="17"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
+      <c r="H27" s="18"/>
+      <c r="I27" s="18"/>
+      <c r="J27" s="18"/>
+      <c r="K27" s="18"/>
     </row>
     <row r="28" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="8" t="s">
@@ -4044,11 +4967,11 @@
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D30" s="18" t="s">
+      <c r="D30" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="E30" s="18"/>
-      <c r="F30" s="18"/>
+      <c r="E30" s="19"/>
+      <c r="F30" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -4069,7 +4992,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K30"/>
   <sheetViews>
@@ -4094,26 +5017,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="16" t="s">
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="16"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
     </row>
     <row r="2" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="19"/>
+      <c r="A2" s="20"/>
       <c r="B2" s="3" t="s">
         <v>22</v>
       </c>
@@ -4146,7 +5069,7 @@
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="19"/>
+      <c r="A3" s="20"/>
       <c r="B3" s="14">
         <v>711</v>
       </c>
@@ -4179,7 +5102,7 @@
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="19"/>
+      <c r="A4" s="20"/>
       <c r="B4" s="14">
         <v>535</v>
       </c>
@@ -4212,7 +5135,7 @@
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="19"/>
+      <c r="A5" s="20"/>
       <c r="B5" s="14">
         <v>535</v>
       </c>
@@ -4245,7 +5168,7 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="19"/>
+      <c r="A6" s="20"/>
       <c r="B6" s="14">
         <v>557</v>
       </c>
@@ -4278,7 +5201,7 @@
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="19"/>
+      <c r="A7" s="20"/>
       <c r="B7" s="14">
         <v>535</v>
       </c>
@@ -4311,7 +5234,7 @@
       </c>
     </row>
     <row r="8" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="19"/>
+      <c r="A8" s="20"/>
       <c r="B8" s="2">
         <f t="shared" ref="B8:K8" si="0">AVERAGE(B3:B7)</f>
         <v>574.6</v>
@@ -4358,26 +5281,26 @@
       <c r="C9" s="14"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="19" t="s">
+      <c r="A10" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="B10" s="20" t="s">
+      <c r="B10" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="20"/>
-      <c r="D10" s="20"/>
-      <c r="E10" s="20"/>
-      <c r="F10" s="20"/>
-      <c r="G10" s="16" t="s">
+      <c r="C10" s="21"/>
+      <c r="D10" s="21"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="21"/>
+      <c r="G10" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="H10" s="16"/>
-      <c r="I10" s="16"/>
-      <c r="J10" s="16"/>
-      <c r="K10" s="16"/>
+      <c r="H10" s="17"/>
+      <c r="I10" s="17"/>
+      <c r="J10" s="17"/>
+      <c r="K10" s="17"/>
     </row>
     <row r="11" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="19"/>
+      <c r="A11" s="20"/>
       <c r="B11" s="3" t="s">
         <v>22</v>
       </c>
@@ -4410,7 +5333,7 @@
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="19"/>
+      <c r="A12" s="20"/>
       <c r="B12" s="14">
         <v>746</v>
       </c>
@@ -4443,7 +5366,7 @@
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="19"/>
+      <c r="A13" s="20"/>
       <c r="B13" s="14">
         <v>673</v>
       </c>
@@ -4476,7 +5399,7 @@
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="19"/>
+      <c r="A14" s="20"/>
       <c r="B14" s="14">
         <v>568</v>
       </c>
@@ -4509,7 +5432,7 @@
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="19"/>
+      <c r="A15" s="20"/>
       <c r="B15" s="14">
         <v>613</v>
       </c>
@@ -4542,7 +5465,7 @@
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="19"/>
+      <c r="A16" s="20"/>
       <c r="B16" s="14">
         <v>568</v>
       </c>
@@ -4575,7 +5498,7 @@
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="19"/>
+      <c r="A17" s="20"/>
       <c r="B17" s="2">
         <f t="shared" ref="B17:K17" si="1">AVERAGE(B12:B16)</f>
         <v>633.6</v>
@@ -4658,20 +5581,20 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="7"/>
-      <c r="B21" s="15" t="s">
+      <c r="B21" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="15"/>
-      <c r="D21" s="15"/>
-      <c r="E21" s="15"/>
-      <c r="F21" s="15"/>
-      <c r="G21" s="16" t="s">
+      <c r="C21" s="16"/>
+      <c r="D21" s="16"/>
+      <c r="E21" s="16"/>
+      <c r="F21" s="16"/>
+      <c r="G21" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="H21" s="16"/>
-      <c r="I21" s="16"/>
-      <c r="J21" s="16"/>
-      <c r="K21" s="16"/>
+      <c r="H21" s="17"/>
+      <c r="I21" s="17"/>
+      <c r="J21" s="17"/>
+      <c r="K21" s="17"/>
     </row>
     <row r="22" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="7"/>
@@ -4842,18 +5765,18 @@
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B27" s="17" t="s">
+      <c r="B27" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="C27" s="17"/>
-      <c r="D27" s="17"/>
-      <c r="E27" s="17"/>
-      <c r="F27" s="17"/>
-      <c r="G27" s="17"/>
-      <c r="H27" s="17"/>
-      <c r="I27" s="17"/>
-      <c r="J27" s="17"/>
-      <c r="K27" s="17"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
+      <c r="H27" s="18"/>
+      <c r="I27" s="18"/>
+      <c r="J27" s="18"/>
+      <c r="K27" s="18"/>
     </row>
     <row r="28" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="8" t="s">
@@ -4946,11 +5869,11 @@
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D30" s="18" t="s">
+      <c r="D30" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="E30" s="18"/>
-      <c r="F30" s="18"/>
+      <c r="E30" s="19"/>
+      <c r="F30" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -4971,12 +5894,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5045,23 +5968,23 @@
         <v>5</v>
       </c>
       <c r="B3" s="1">
-        <f>ORMLite!B7</f>
+        <f>ORMLite!B8</f>
         <v>8422.7999999999993</v>
       </c>
       <c r="C3" s="1">
-        <f>ORMLite!C7</f>
+        <f>ORMLite!C8</f>
         <v>8430.6</v>
       </c>
       <c r="D3" s="1">
-        <f>ORMLite!D7</f>
+        <f>ORMLite!D8</f>
         <v>449.8</v>
       </c>
       <c r="E3" s="1">
-        <f>ORMLite!E7</f>
+        <f>ORMLite!E8</f>
         <v>456.6</v>
       </c>
       <c r="F3" s="1">
-        <f>ORMLite!F7</f>
+        <f>ORMLite!F8</f>
         <v>358.4</v>
       </c>
     </row>
@@ -5162,7 +6085,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K29"/>
   <sheetViews>
@@ -5187,26 +6110,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="16" t="s">
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="16"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
     </row>
     <row r="2" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="19"/>
+      <c r="A2" s="20"/>
       <c r="B2" s="3" t="s">
         <v>22</v>
       </c>
@@ -5239,7 +6162,7 @@
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="19"/>
+      <c r="A3" s="20"/>
       <c r="D3" s="11"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
@@ -5251,7 +6174,7 @@
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="19"/>
+      <c r="A4" s="20"/>
       <c r="D4" s="11"/>
       <c r="E4" s="11"/>
       <c r="F4" s="11"/>
@@ -5263,7 +6186,7 @@
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="19"/>
+      <c r="A5" s="20"/>
       <c r="D5" s="11"/>
       <c r="E5" s="11"/>
       <c r="F5" s="11"/>
@@ -5275,7 +6198,7 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="19"/>
+      <c r="A6" s="20"/>
       <c r="D6" s="11"/>
       <c r="E6" s="11"/>
       <c r="F6" s="11"/>
@@ -5287,7 +6210,7 @@
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="19"/>
+      <c r="A7" s="20"/>
       <c r="D7" s="11"/>
       <c r="E7" s="11"/>
       <c r="F7" s="11"/>
@@ -5299,7 +6222,7 @@
       </c>
     </row>
     <row r="8" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="19"/>
+      <c r="A8" s="20"/>
       <c r="B8" s="2" t="e">
         <f t="shared" ref="B8:K8" si="0">AVERAGE(B3:B7)</f>
         <v>#DIV/0!</v>
@@ -5342,33 +6265,33 @@
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D9" s="18" t="s">
+      <c r="D9" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="19"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="19" t="s">
+      <c r="A10" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="B10" s="15" t="s">
+      <c r="B10" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="15"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="16" t="s">
+      <c r="C10" s="16"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="H10" s="16"/>
-      <c r="I10" s="16"/>
-      <c r="J10" s="16"/>
-      <c r="K10" s="16"/>
+      <c r="H10" s="17"/>
+      <c r="I10" s="17"/>
+      <c r="J10" s="17"/>
+      <c r="K10" s="17"/>
     </row>
     <row r="11" spans="1:11" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="19"/>
+      <c r="A11" s="20"/>
       <c r="B11" s="3" t="s">
         <v>22</v>
       </c>
@@ -5401,7 +6324,7 @@
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="19"/>
+      <c r="A12" s="20"/>
       <c r="D12" s="11"/>
       <c r="E12" s="11"/>
       <c r="F12" s="11"/>
@@ -5422,7 +6345,7 @@
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="19"/>
+      <c r="A13" s="20"/>
       <c r="D13" s="11"/>
       <c r="E13" s="11"/>
       <c r="F13" s="11"/>
@@ -5443,7 +6366,7 @@
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="19"/>
+      <c r="A14" s="20"/>
       <c r="D14" s="11"/>
       <c r="E14" s="11"/>
       <c r="F14" s="11"/>
@@ -5464,7 +6387,7 @@
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="19"/>
+      <c r="A15" s="20"/>
       <c r="D15" s="11"/>
       <c r="E15" s="11"/>
       <c r="F15" s="11"/>
@@ -5485,7 +6408,7 @@
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="19"/>
+      <c r="A16" s="20"/>
       <c r="D16" s="11"/>
       <c r="E16" s="11"/>
       <c r="F16" s="11"/>
@@ -5506,7 +6429,7 @@
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="19"/>
+      <c r="A17" s="20"/>
       <c r="B17" s="2" t="e">
         <f t="shared" ref="B17:J17" si="1">AVERAGE(B12:B16)</f>
         <v>#DIV/0!</v>
@@ -5552,11 +6475,11 @@
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
-      <c r="D18" s="18" t="s">
+      <c r="D18" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="E18" s="18"/>
-      <c r="F18" s="18"/>
+      <c r="E18" s="19"/>
+      <c r="F18" s="19"/>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
@@ -5591,20 +6514,20 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="7"/>
-      <c r="B21" s="15" t="s">
+      <c r="B21" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="15"/>
-      <c r="D21" s="15"/>
-      <c r="E21" s="15"/>
-      <c r="F21" s="15"/>
-      <c r="G21" s="16" t="s">
+      <c r="C21" s="16"/>
+      <c r="D21" s="16"/>
+      <c r="E21" s="16"/>
+      <c r="F21" s="16"/>
+      <c r="G21" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="H21" s="16"/>
-      <c r="I21" s="16"/>
-      <c r="J21" s="16"/>
-      <c r="K21" s="16"/>
+      <c r="H21" s="17"/>
+      <c r="I21" s="17"/>
+      <c r="J21" s="17"/>
+      <c r="K21" s="17"/>
     </row>
     <row r="22" spans="1:11" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="7"/>
@@ -5824,7 +6747,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K25"/>
   <sheetViews>
@@ -5849,26 +6772,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="16" t="s">
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="16"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
     </row>
     <row r="2" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="19"/>
+      <c r="A2" s="20"/>
       <c r="B2" s="3" t="s">
         <v>22</v>
       </c>
@@ -5901,7 +6824,7 @@
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="19"/>
+      <c r="A3" s="20"/>
       <c r="B3" s="1">
         <v>602</v>
       </c>
@@ -5934,7 +6857,7 @@
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="19"/>
+      <c r="A4" s="20"/>
       <c r="B4" s="1">
         <v>599</v>
       </c>
@@ -5967,7 +6890,7 @@
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="19"/>
+      <c r="A5" s="20"/>
       <c r="B5" s="1">
         <v>738</v>
       </c>
@@ -6000,7 +6923,7 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="19"/>
+      <c r="A6" s="20"/>
       <c r="B6" s="1">
         <v>729</v>
       </c>
@@ -6033,7 +6956,7 @@
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="19"/>
+      <c r="A7" s="20"/>
       <c r="B7" s="1">
         <v>757</v>
       </c>
@@ -6066,7 +6989,7 @@
       </c>
     </row>
     <row r="8" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="19"/>
+      <c r="A8" s="20"/>
       <c r="B8" s="2">
         <f t="shared" ref="B8:K8" si="0">AVERAGE(B3:B7)</f>
         <v>685</v>
@@ -6109,33 +7032,33 @@
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D9" s="18" t="s">
+      <c r="D9" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="19"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="19" t="s">
+      <c r="A10" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="B10" s="15" t="s">
+      <c r="B10" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="15"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="16" t="s">
+      <c r="C10" s="16"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="H10" s="16"/>
-      <c r="I10" s="16"/>
-      <c r="J10" s="16"/>
-      <c r="K10" s="16"/>
+      <c r="H10" s="17"/>
+      <c r="I10" s="17"/>
+      <c r="J10" s="17"/>
+      <c r="K10" s="17"/>
     </row>
     <row r="11" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="19"/>
+      <c r="A11" s="20"/>
       <c r="B11" s="3" t="s">
         <v>22</v>
       </c>
@@ -6168,7 +7091,7 @@
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="19"/>
+      <c r="A12" s="20"/>
       <c r="B12" s="1">
         <v>790</v>
       </c>
@@ -6201,7 +7124,7 @@
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="19"/>
+      <c r="A13" s="20"/>
       <c r="B13" s="1">
         <v>649</v>
       </c>
@@ -6234,7 +7157,7 @@
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="19"/>
+      <c r="A14" s="20"/>
       <c r="B14" s="1">
         <v>634</v>
       </c>
@@ -6267,7 +7190,7 @@
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="19"/>
+      <c r="A15" s="20"/>
       <c r="B15" s="1">
         <v>635</v>
       </c>
@@ -6300,7 +7223,7 @@
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="19"/>
+      <c r="A16" s="20"/>
       <c r="B16" s="1">
         <v>628</v>
       </c>
@@ -6333,7 +7256,7 @@
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="19"/>
+      <c r="A17" s="20"/>
       <c r="B17" s="2">
         <f t="shared" ref="B17:K17" si="1">AVERAGE(B12:B16)</f>
         <v>667.2</v>
@@ -6379,11 +7302,11 @@
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
-      <c r="D18" s="18" t="s">
+      <c r="D18" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="E18" s="18"/>
-      <c r="F18" s="18"/>
+      <c r="E18" s="19"/>
+      <c r="F18" s="19"/>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
@@ -6418,20 +7341,20 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="7"/>
-      <c r="B21" s="15" t="s">
+      <c r="B21" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="15"/>
-      <c r="D21" s="15"/>
-      <c r="E21" s="15"/>
-      <c r="F21" s="15"/>
-      <c r="G21" s="16" t="s">
+      <c r="C21" s="16"/>
+      <c r="D21" s="16"/>
+      <c r="E21" s="16"/>
+      <c r="F21" s="16"/>
+      <c r="G21" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="H21" s="16"/>
-      <c r="I21" s="16"/>
-      <c r="J21" s="16"/>
-      <c r="K21" s="16"/>
+      <c r="H21" s="17"/>
+      <c r="I21" s="17"/>
+      <c r="J21" s="17"/>
+      <c r="K21" s="17"/>
     </row>
     <row r="22" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="7"/>
@@ -6617,7 +7540,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G15"/>
   <sheetViews>
@@ -6691,23 +7614,23 @@
         <v>5</v>
       </c>
       <c r="B3" s="1">
-        <f>ORMLite!B7</f>
+        <f>ORMLite!B8</f>
         <v>8422.7999999999993</v>
       </c>
       <c r="C3" s="1">
-        <f>ORMLite!C7</f>
+        <f>ORMLite!C8</f>
         <v>8430.6</v>
       </c>
       <c r="D3" s="1">
-        <f>ORMLite!D7</f>
+        <f>ORMLite!D8</f>
         <v>449.8</v>
       </c>
       <c r="E3" s="1">
-        <f>ORMLite!E7</f>
+        <f>ORMLite!E8</f>
         <v>456.6</v>
       </c>
       <c r="F3" s="1">
-        <f>ORMLite!F7</f>
+        <f>ORMLite!F8</f>
         <v>358.4</v>
       </c>
     </row>
@@ -6818,7 +7741,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H10"/>
   <sheetViews>
@@ -7029,150 +7952,4 @@
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:F7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="11.42578125" style="1"/>
-    <col min="2" max="2" width="13.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="11.42578125" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B2" s="1">
-        <v>8540</v>
-      </c>
-      <c r="C2" s="1">
-        <v>8895</v>
-      </c>
-      <c r="D2" s="1">
-        <v>426</v>
-      </c>
-      <c r="E2" s="1">
-        <v>414</v>
-      </c>
-      <c r="F2" s="1">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B3" s="1">
-        <v>8575</v>
-      </c>
-      <c r="C3" s="1">
-        <v>8117</v>
-      </c>
-      <c r="D3" s="1">
-        <v>506</v>
-      </c>
-      <c r="E3" s="1">
-        <v>489</v>
-      </c>
-      <c r="F3" s="1">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B4" s="1">
-        <v>7593</v>
-      </c>
-      <c r="C4" s="1">
-        <v>8881</v>
-      </c>
-      <c r="D4" s="1">
-        <v>428</v>
-      </c>
-      <c r="E4" s="1">
-        <v>446</v>
-      </c>
-      <c r="F4" s="1">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B5" s="1">
-        <v>9451</v>
-      </c>
-      <c r="C5" s="1">
-        <v>7448</v>
-      </c>
-      <c r="D5" s="1">
-        <v>436</v>
-      </c>
-      <c r="E5" s="1">
-        <v>498</v>
-      </c>
-      <c r="F5" s="1">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B6" s="1">
-        <v>7955</v>
-      </c>
-      <c r="C6" s="1">
-        <v>8812</v>
-      </c>
-      <c r="D6" s="1">
-        <v>453</v>
-      </c>
-      <c r="E6" s="1">
-        <v>436</v>
-      </c>
-      <c r="F6" s="1">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="2">
-        <f>AVERAGE(B2:B6)</f>
-        <v>8422.7999999999993</v>
-      </c>
-      <c r="C7" s="2">
-        <f>AVERAGE(C2:C6)</f>
-        <v>8430.6</v>
-      </c>
-      <c r="D7" s="2">
-        <f>AVERAGE(D2:D6)</f>
-        <v>449.8</v>
-      </c>
-      <c r="E7" s="2">
-        <f>AVERAGE(E2:E6)</f>
-        <v>456.6</v>
-      </c>
-      <c r="F7" s="2">
-        <f>AVERAGE(F2:F6)</f>
-        <v>358.4</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>